<commit_message>
(v2.1.1.9217) allow + in amr selectors
</commit_message>
<xml_diff>
--- a/data-raw/antimicrobials.xlsx
+++ b/data-raw/antimicrobials.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>aminopar,aminosalicylic,aminosalicylicacid,aminosalyl,aminox,apacil,deapasil,entepas,ferrosan,gabbropas,granupas,helipidyl,hellipidyl,neopasalate,osacyl,pamacyl,pamisyl,paramycin,parasal,parasalicil,parasalindon,pasalon,pasara,pascorbic,pasdium,pasergranules,paskalium,pasmed,pasnodia,pasolac,propasa,rezipas,teebacin</t>
+          <t>aminacyl,aminopar,aminosalicylate,aminosalicylic,aminosalyl,aminox,apacil,deapasil,entepas,gabbropas,granupas,helipidyl,hellipidyl,nemasol,nippas,osacyl,pamacyl,pamisyl,paramisan,paramycin,parasal,parasalicil,parasalindon,pasade,pasalon,pasara,pascorbic,pasdium,pasem,paser,pasmed,pasnal,pasnodia,pasolac,passodico,pharmakon,propasa,rezipas,salvis,sanipirol,sanipriol,sodiopas,spectrum</t>
         </is>
       </c>
       <c r="J2">
@@ -604,7 +604,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>foromacidinb,spiramycinii</t>
+          <t>antibiotic,espiramicin,espiramicina,foromacidin,provamycin,rovamicina,rovamycin,rovamycine,selectomycin,sequamycin,spiramycine,spiramycinum</t>
         </is>
       </c>
       <c r="J4" t="e">
@@ -666,7 +666,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>adesulfonesodium,aldapsone,aldesulfonasodica,aldesulfone,aldesulfonesodique,aldesulfonesodium,aldesulphonesodium,diamidin,diasone,diasonesodium,diazon,novotrone,sodiumaldesulphone,sodiumsulfoxone,sulfoxonesodium</t>
+          <t>adesulfone,aldapsone,aldesulfone,aldesulphone,diamidin,diason,diasone,diasoneenterab,diazon,didimethanesulfinate,novotrone,sulfoxone</t>
         </is>
       </c>
       <c r="J5">
@@ -730,7 +730,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>amicacin,amikacillin,amikacina,amikacinbase,amikacindihydrate,amikacine,amikacinfreebase,amikacinsulfate,amikacinum,amikavet,amikin,amiklin,amikozit,amukin,arikace,arikayceliposomal,briclin,kaminax,lukadin,mikavir,pierami,potentox</t>
+          <t>amicacin,amikacillin,amikacina,amikacine,amikacinum,amikavet,amikin,amikozit,amukin,arikace,briclin,butirosins,kaminax,lukadin,mikavir,potentox,prestwick</t>
         </is>
       </c>
       <c r="J6" t="e">
@@ -852,7 +852,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>amorolfina,amorolfinum,loceryl</t>
+          <t>amorolfina,amorolfinum,bekiron,corbel,curanail,fenpropemorph,fenpropimorph,fenpropimorphe,forbel,funbas,loceryl,locetar,mildofix,mistral,morpholine,odenil,omicur,pekiron</t>
         </is>
       </c>
       <c r="J8" t="e">
@@ -914,7 +914,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>actimoxi,amoclen,amolin,amopen,amopenixin,amoxibiotic,amoxicaps,amoxicilina,amoxicilline,amoxicillinhydrate,amoxicillinum,amoxiden,amoxil,amoxivet,amoxy,amoxycillin,amoxyke,anemolin,aspenil,atoksilin,biomox,bristamox,cemoxin,clamoxyl,damoxy,delacillin,demoksil,dispermox,efpenix,flemoxin,hiconcil,histocillin,hydroxyampicillin,ibiamox,imacillin,lamoxy,largopen,metafarmacapsules,metifarmacapsules,moksilin,moxacin,moxatag,ospamox,pamoxicillin,piramox,promoxil,remoxil,robamox,sawamoxpm,tolodina,topramoxin,unicillin,utimox,vetramox</t>
+          <t>acuotricina,alfamox,alfida,amitron,amoclen,amodex,amoksicillin,amolin,amopen,amopenixin,amophar,amoran,amoxi,amoxicaps,amoxicilina,amoxicilline,amoxicillinum,amoxidal,amoxiden,amoxil,amoxillat,amoxina,amoxine,amoxipen,amoxivet,amoxycillin,amoxycillinsalt,amoxyke,anemolin,aspenil,atoksilin,bristamox,cemoxin,ciblor,clamoxyl,damoxy,danoxillin,delacillin,demoksil,dispermox,efpenix,eupen,flemoxin,flemoxine,galenamox,gramidil,hiconcil,himinomax,histocillin,ibiamox,imacillin,izoltil,kentrocyllin,lamoxy,largopen,larotid,matasedrin,metifarma,moksilin,moxacin,moxal,moxaline,moxatag,neotetranase,novabritine,ospamox,pacetocin,pamocil,paradroxil,pasetocin,penamox,piramox,promoxil,quimiopen,remoxil,riotapen,robamox,sawacillin,siganopen,simplamox,sintopen,sumox,topramoxin,trifamox,trimox,unicillin,utimox,velamox,vetramox,wymox,zamocillin,zamocilline,zimox</t>
         </is>
       </c>
       <c r="J9">
@@ -980,7 +980,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>amocla,amoclan,amoclav,amoksiclav,amoxsiklav,amoxyclav,augmentan,augmentin,augmentine,augmentinxr,auspilic,clamentin,clamobit,clavamox,clavinex,clavoxilinplus,clavulin,clavumox,coamoxiclav,eumetinex,kmoxilin,spectramox,spektramox,synulox,viaclav,xiclav</t>
+          <t>amocla,amoclan,amoclav,amoksiclav,amoxsiklav,amoxyclav,ancla,augmentan,augmentin,augmentine,auspilic,clamentin,clamobit,clavam,clavamox,clavinex,clavumox,coamoxiclav,curam,eumetinex,kesium,kmoxilin,spectramox,synulox,viaclav,xiclav</t>
         </is>
       </c>
       <c r="J10">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>abelcet,abelecet,ambisome,amfotericinab,amphocin,amphomoronal,amphortericinb,amphotec,amphotericin,amphotericinb,amphotericineb,amphotericinumb,amphozone,anfotericineb,fungilin,fungisome,fungisone,fungizone,halizon</t>
+          <t>abelcet,abelecet,ambil,ambisome,amphocin,amphomoronal,amphotec,amphotericin,amphotocerin,amphozone,funganiline,fungilin,fungisome,fungisone,fungizone,halizon,nystatine,nystatinum,terrastatin</t>
         </is>
       </c>
       <c r="J12">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>acillin,adobacillin,amblosin,amcill,amfipen,amfipenv,amipenixs,ampichel,ampicil,ampicilina,ampicillina,ampicillinacid,ampicillinanhydrate,ampicillinanhydrous,ampicillinbase,ampicilline,ampicillinhydrate,ampicillinsodium,ampicillinum,ampicin,ampifarm,ampikel,ampimed,ampipenin,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,anhydrousampicillin,austrapen,binotal,bonapicillin,britacil,campicillin,copharcilin,delcillin,deripen,divercillin,doktacillin,duphacillin,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,olinkid,omnipen,orbicilina,penampil,penaoral,penbristol,penbritin,penbritinpaediatric,penbritinsyrup,penbrock,penicline,penimic,pensyn,pentrex,pentrexl,pentrexyl,pentritin,pfizerpena,polycillin,polyflex,ponecil,princillin,principen,qidamp,racenacillin,redicilin,rosampline,roscillin,semicillin,semicillinr,servicillin,sumipanto,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,viccillins,vidocillin,wypicil</t>
+          <t>acillin,adobacillin,alpen,amblosin,amcap,amcill,amfipen,ampen,amperil,ampichel,ampicil,ampicilina,ampicillina,ampicilline,ampicillinesalt,ampicillinsalt,ampicillinum,ampicin,ampifarm,ampikel,ampimed,ampinova,ampipenin,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,austrapen,bayer,binotal,bonapicillin,britacil,campicillin,cimex,citteral,copharcilin,cymbi,delcillin,deripen,divercillin,doktacillin,domicillin,duphacillin,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,omnipen,orbicilina,penbristol,penbritin,penbrock,penialmen,penicillin,penicline,penimic,penizillin,pensyn,pentrex,pentrexl,pentrexyl,pentritin,ponecil,princillin,principen,racenacillin,redicilin,rosampline,roscillin,semicillin,servicillin,sumipanto,supen,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trafarbiot,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,vidocillin,wypicil</t>
         </is>
       </c>
       <c r="J14">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>amprocidum,amprol,amprolio,amproliumchloride,amprovine,thiacoccid</t>
+          <t>amprol,amprolio,amprovine,anticoccid,cocciprol,corid,mepyrium,picolinium,pyridinium,thiacoccid</t>
         </is>
       </c>
       <c r="J16" t="e">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>anidulafungina,anidulafungine,anidulafunginum,ecalta,eraxis</t>
+          <t>anidulafungina,anidulafungine,anidulafunginum,biafungin,ecalta,eraxis</t>
         </is>
       </c>
       <c r="J17" t="e">
@@ -1476,7 +1476,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>apalcilina,apalcilline,apalcillinum</t>
+          <t>apalcilina,apalcilline,apalcillinsalt,apalcillinum,lumota</t>
         </is>
       </c>
       <c r="J18" t="e">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>ambylan,apralan,apramicina,apramycine,apramycinum,nebramycinii</t>
+          <t>ambylan,apralan,apramicina,apramycine,apramycinum</t>
         </is>
       </c>
       <c r="J19" t="e">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>arbekacina,arbekacine,arbekacinisulfas,arbekacinum,haberacin</t>
+          <t>arbekacina,arbekacine,arbekacinum,haberacin</t>
         </is>
       </c>
       <c r="J20" t="e">
@@ -1652,7 +1652,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>aspoxicilina,aspoxicillan,aspoxicilline,aspoxicillinum</t>
+          <t>aspoxicilina,aspoxicillan,aspoxicilline,aspoxicillinum,doyle</t>
         </is>
       </c>
       <c r="J21" t="e">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>astromicina,astromicine,astromicinum,fortimicin,fortimicina</t>
+          <t>abbott,astromicina,astromicine,astromicinum,fortimicin,istamycin,istamycins</t>
         </is>
       </c>
       <c r="J22" t="e">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>avilamycina,avilamycine,avilamycinum,surmax</t>
+          <t>avilamycina,avilamycine,avilamycinum,inteprity,kavault,surmax</t>
         </is>
       </c>
       <c r="J24" t="e">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>avoparcina,avoparcine,avoparcinum,avotan</t>
+          <t>firvanq,tagocid,targocid,targosid,tecoplanina,tecoplanine,tecoplaninum,teichomycin,teicoplanina,teicoplanine,teicoplaninum,teikoplanin,ticocin</t>
         </is>
       </c>
       <c r="J25" t="e">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>aritromicina,aruzilina,azasite,azenil,azifast,azigram,azimakrol,azithramycine,azithrocin,azithromycine,azithromycinum,azitrocin,azitromax,azitromicina,azitromicine,azitromin,aziwin,aziwok,aztrin,azyter,azythromycin,durasite,hemomycin,macrozit,misultina,mixoterin,setron,sumamed,toraseptol,tromix,trozocina,trulimax,xithrone,zentavion,zithrax,zithromac,zithromax,zithromaxiv,zithromycin,zitrim,zitromax,zitrotek,zmaxsr,zythromax</t>
+          <t>aritromicina,aruzilina,azasite,azenil,azifast,azigram,azimakrol,azithramycine,azithrocin,azithromycine,azithromycinum,azitrocin,azitromax,azitromicina,azitromicine,azitromin,aziwin,aziwok,aztrin,azyter,hemomycin,macrozit,misultina,mixoterin,setron,sumamed,tobil,toraseptol,tromix,trozocina,trulimax,xithrone,zentavion,zifin,zithrax,zithromac,zithromax,zithromycin,zitrim,zitromax,zitrotek,zythromax</t>
         </is>
       </c>
       <c r="J27">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>azlocilina,azlocilline,azlocillinum</t>
+          <t>azlin,azlocilina,azlocilline,azlocillinsalt,azlocillinum,securopen</t>
         </is>
       </c>
       <c r="J29" t="e">
@@ -2204,7 +2204,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>azactam,azetreonam,azonam,azthreonam,aztreon,nebactam,primbactam</t>
+          <t>azactam,azetreonam,azonam,azthreonam,aztreon,aztreonamum,cayston,dynabiotic,nebactam,primbactam,squibb</t>
         </is>
       </c>
       <c r="J30" t="e">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>bacampicilina,bacampicilline,bacampicillinum,penglobe</t>
+          <t>alphacilina,alphacillin,ambacamp,ambaxin,bacacil,bacampicilina,bacampicilline,bacampicillinum,bacampicine,berocillin,centurina,devonium,diancina,inacilin,maxifen,penglobe,pivatil,pondocil,pondocillin,pondocillina,sanguicillin,spectrobid,velbacil</t>
         </is>
       </c>
       <c r="J33">
@@ -2444,7 +2444,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>fortracin,mdbacitracin</t>
+          <t>albac,altracin,ayfivin,baciferm,baciguent,baciim,baciliquin,bacilliquin,baciquent,bacitracina,bacitracine,bacitracinum,citracin,fortracin,mycitracin,parentracin,penitracin,septa,topitracin,topitrasin,tropitracin,zutracin</t>
         </is>
       </c>
       <c r="J34" t="e">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>sirturo</t>
+          <t/>
         </is>
       </c>
       <c r="J35">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>aminodeoxykanamycin,becanamicina,bekanamycine,bekanamycinum,kanamycinb,klebcil,nebramycinv</t>
+          <t>aminodeoxykanamycin,becanamicina,bekanamicina,bekanamycine,bekanamycinum</t>
         </is>
       </c>
       <c r="J36" t="e">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>beacillin,cepacilina,extencilline,lentopenil,penidural,tardocillin</t>
+          <t/>
         </is>
       </c>
       <c r="J37" t="e">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>bicillinv,biphecillin</t>
+          <t>bicillin,biphecillin</t>
         </is>
       </c>
       <c r="J38">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>abbocillin,ayercillin,bencilpenicilina,benzopenicillin,benzylpenicilline,benzylpenicilling,benzylpenicillinum,bicillin,cillora,cilloral,cilopen,compocilling,cosmopen,dropcillin,freepenicilling,freepenicillinii,galofak,gelacillin,liquacillin,megacillin,pencilling,penicillin,penicilling,pentids,permapen,pfizerpen,pfizerpeng,pharmacillin,pradupen,specillineg,ursopen</t>
+          <t>bencilpenicilina,benzopenicillin,benzylpenicilline,benzylpenicillinum,capicillin,cillora,cilloral,cilopen,cintrisul,cosmopen,cristapen,crystapen,dropcillin,eskacillin,ethacillin,falapen,forpen,galofak,gelacillin,hipercilina,hyasorb,hylenta,lemopen,liquacillin,liquapen,monocillin,monopen,mycofarm,novocillin,penalev,penicillinum,penilaryn,penisem,pentid,pentids,pfizerpen,pharmacillin,pradupen,scotcil,sugracillin,sugracillinsalt,tabilin,ursopen,veticillin</t>
         </is>
       </c>
       <c r="J39" t="e">
@@ -2896,7 +2896,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BTL-S</t>
+          <t>BLA-S</t>
         </is>
       </c>
       <c r="B42" t="e">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>biapenern,bipenem,omegacin</t>
+          <t>biapenern,omegacin</t>
         </is>
       </c>
       <c r="J43" t="e">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>ble,bleo</t>
+          <t>blenamax,blenoxane,bleocin,bleomicin,bleomicina,bleomycine,bleomycins,bleomycinum,blexane,nbleomycinamide</t>
         </is>
       </c>
       <c r="J45" t="e">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>butaconazole,butoconazol,butoconazolum,compositenstarke,dahlin,femstat,gynofort,polyfructosanum</t>
+          <t>butaconazole,butoconazol,butoconazolum,gynofort</t>
         </is>
       </c>
       <c r="J47" t="e">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>anabactyl,carbenicilina,carbenicillina,carbenicilline,carbenicillinum,geopen,pyopen</t>
+          <t>anabactyl,carbecin,carbenicilina,carbenicillina,carbenicilline,carbenicillinum,dicarbenicillin,dipenicillin,fugacillin,geopen,gripenin,hyoper,microcillin,piopen,pyocianil,pyoclox,pyopan,pyopen,pyopene</t>
         </is>
       </c>
       <c r="J51" t="e">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>carindacilina,carindacilline,carindacillinum</t>
+          <t>carindacilina,carindacilline,carindacillinsalt,carindacillinum,geocillin,indanylcarbinicillin,urobac</t>
         </is>
       </c>
       <c r="J52">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>cancidas,capsofungin</t>
+          <t>cancidas,caspofungina</t>
         </is>
       </c>
       <c r="J54" t="e">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>cefacetril,cefacetrilo,cefacetrilum,celospor,celtol,cephacetrile,cristacef,vetrimast</t>
+          <t>cefacetril,cefacetrilo,cefacetrilum,celospor,cephacetrile,vetrimast</t>
         </is>
       </c>
       <c r="J55" t="e">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>alenfral,alfacet,ceclor,ceclorcd,cefacloranhydrous,cefaclorimpurityc,cefaclormonohydrate,cefacloro,cefaclorum,cefeaclor,cephaclor,dystaclormr,keflor,kefral,panoral,raniclor</t>
+          <t>alenfral,alfacet,alfatil,ceclor,cefachlor,cefaclorum,cefeaclor,cephaclor,cephalexin,compound,distaclor,keflor,kefolor,kefral,keftab,keftid,lilly,lopac,panacef,panoral,raniclor</t>
         </is>
       </c>
       <c r="J56">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>anhydrouscefadroxil,cefadrops,cefadroxilanhydrous,cefadroxilo,cefadroxilum,cefradroxil,cephadroxil,duracef,duricef,sumacef,ultracef</t>
+          <t>bidocel,cefadrops,cefadroxilo,cefadroxilum,cefradroxil,cefzil,cephadroxil,duracef,duricef,kefroxil,sumacef,ultracef</t>
         </is>
       </c>
       <c r="J57">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>alcephin,alexin,alsporin,amplex,anhydrouscefalexin,anhydrouscephalexin,biocef,carnosporin,cefablan,cefadal,cefadin,cefadina,cefaleksin,cefalessina,cefalexina,cefalexinanhydrous,cefalexine,cefalexinum,cefalin,cefaloto,cefaseptin,ceffanex,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalexin,cephalexinanhydrous,cephalexine,cephalexinum,cephanasten,cephaxin,cephin,ceporex,ceporexforte,ceporexin,ceporexine,cerexin,cerexins,cophalexin,durantel,durantelds,erocetin,factagard,felexin,ibilex,ibrexin,inphalex,kefalospes,keflet,keflex,kefolan,keforal,keftab,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,lonflex,lopilexin,madlexin,mamalexin,mamlexin,medoxine,neokef,neolexina,novolexin,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panixinedisperdose,pectril,pyassan,roceph,rocephdistab,sanaxin,sartosona,sencephalin,sepexin,servispor,sialexin,sinthecillin,sporicef,sporidex,syncle,synecl,tepaxin,tokiolexin,uphalexin,voxxim,winlex,zozarine</t>
+          <t>adcadina,alcephin,alexin,alsporin,ambal,amplex,aristosporin,azabort,bactopenor,beliam,biocef,carnosporin,cefablan,cefacet,cefadal,cefadin,cefadina,cefalekey,cefaleksin,cefalessina,cefalexgobens,cefalexina,cefalexine,cefalexinum,cefalin,cefalival,cefaloto,cefanex,cefaseptin,cefax,ceffanex,cefibacter,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalexine,cephalexinum,cephalobene,cephanasten,cephaxin,cephin,cepol,ceporex,ceporexin,ceporexine,cerexin,cerexins,check,cophalexin,domucef,doriman,durantel,efemida,erocetin,factagard,felexin,fexin,ibilex,ibrexin,inphalex,karilexina,kefalospes,keflet,keflex,kefolan,keforal,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,loisine,lonflex,lopilexin,losporal,madlexin,maksipor,mamalexin,mamlexin,medolexin,medoxine,neokef,neolexina,noveol,novolexin,nufex,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panixine,pectril,prindex,pyassan,rilexine,roceph,rogevil,sanaxin,sartosona,sencephalin,sepexin,servicef,servispor,sialexin,sinthecillin,sintolexyn,sporicef,sporidex,syncl,syncle,synecl,taicelexin,tepaxin,theratrex,tokiolexin,uphalexin,viosporine,voxxim,winlex,zabytrex,zozarine</t>
         </is>
       </c>
       <c r="J58">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>cefalothin,cefalotina,cefalotinafabra,cefalotine,cefalotinum,cemastin,cephalothinum,cephalotin,cephalotinacid,coaxin,keflin,seffin</t>
+          <t>averon,cefalothin,cefalothine,cefalothinsalt,cefalotina,cefalotine,cefalotinsalt,cefalotinum,cemastin,cephalothin,cephalothinsalt,cephalothinum,cephalotin,cephalotinsalt,ceporacin,cepovenin,coaxin,keflin,lospoven,microtin,seffin,synclotin,toricelocin</t>
         </is>
       </c>
       <c r="J60" t="e">
@@ -4110,7 +4110,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>cefadole,cefamandol,cefamandolum,cephadole,cephamandole,kefamandol,kefdole,mancef</t>
+          <t>cefadole,cefamandol,cefamandolum,cephadole,kefamandol,kefdole,mancef</t>
         </is>
       </c>
       <c r="J61" t="e">
@@ -4174,7 +4174,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>ambrocef,cefadyl,cefapilin,cefapirina,cefapirine,cefapirinum,cefaprin,cefaprinsodium,cefatrex,cefatrexyl,cephapirine,metricure</t>
+          <t>ambrocef,brisfirina,brisporin,bristocef,cefadyl,cefalak,cefaloject,cefapirina,cefapirine,cefapirinsalt,cefapirinum,cefaprin,cefatrex,cefatrexyl,cephapirin,cephapirine,cephapirinsalt,cephatrexil,cephatrexyl,metricure</t>
         </is>
       </c>
       <c r="J62" t="e">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>bricef,cefatrix,cefatrizino,cefatrizinum,cephatriazine,cepticol,cetrazil,latocef,orosporina,trizina</t>
+          <t>bricef,cefathiamidine,cefatrix,cefatrizino,cefatrizinum,cephatriazine,cepticol,cetrazil,latocef,orosporina,orotric,seapuron,trizina</t>
         </is>
       </c>
       <c r="J63">
@@ -4302,7 +4302,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>cefazedon,cefazedona,cefazedoneacid,cefazedonum,refosporen,refosporene,refosporin</t>
+          <t>cefazedon,cefazedona,cefazedonesalt,cefazedonum,refosporen,refosporene,refosporin,refosporinsalt</t>
         </is>
       </c>
       <c r="J64" t="e">
@@ -4366,7 +4366,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>atirin,cefamezin,cefamezine,cefazina,cefazolina,cefazolinacid,cefazoline,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,kefzol,liviclina,totacef</t>
+          <t>ancef,atirin,biazolina,cefabiozim,cefacidal,cefalomicina,cefamedin,cefamezin,cefazil,cefazina,cefazolina,cefazoline,cefazolinsalt,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,gramaxin,kefzol,lampocef,liviclina,neofazol,oprea,recef,totacef,zolicef,zolin,zolisint</t>
         </is>
       </c>
       <c r="J65" t="e">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>cefbuperazona,cefbuperazonum,cefbuperzaone,cerbuperazone,tomiporan</t>
+          <t>cefbuperazona,cefbuperazonesalt,cefbuperazonum,cefbuperzaone,cerbuperazone,keiperazon,tomiporan</t>
         </is>
       </c>
       <c r="J66" t="e">
@@ -4486,7 +4486,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>cefcamate</t>
+          <t>flomox</t>
         </is>
       </c>
       <c r="J67">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>cefcamatepivoxil,cefcapenepiroxil</t>
+          <t>cefcamate,flumax</t>
         </is>
       </c>
       <c r="J68" t="e">
@@ -4608,7 +4608,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>cefdiniranhydrous,cefdinirum,cefdinyl,cefdirnir,ceftinex,cefzon,omnicef</t>
+          <t>cefdinirum,cefdinyl,cefdirnir,ceftinex,cefzon,omnicef</t>
         </is>
       </c>
       <c r="J69">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t/>
+          <t>cefditoreno,spectracef</t>
         </is>
       </c>
       <c r="J70">
@@ -4732,7 +4732,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>cefditorenpivoxil,cefditorin,cefditorinpivoxil,meiact,spectracef</t>
+          <t>cefditorin,meiact,pivaloyloxymethyl</t>
         </is>
       </c>
       <c r="J71" t="e">
@@ -4794,7 +4794,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>axepim,cefepima,cefepimum,cepimax,cepimex,maxcef,maxipime</t>
+          <t>anticefepime,axepim,cefepima,cefepimum,maxipime,pyrrolidinium,renapime</t>
         </is>
       </c>
       <c r="J72" t="e">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>cefetametum,cepimeo,deacetoxycefotaxime</t>
+          <t>cefetametum,deacetoxycefotaxime,epocelin</t>
         </is>
       </c>
       <c r="J78">
@@ -5212,7 +5212,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>cefetametpivoxyl,globocef</t>
+          <t>cefetametpivoxil,cefyl,globocef</t>
         </is>
       </c>
       <c r="J79" t="e">
@@ -5270,7 +5270,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>cefetecolanhydrous</t>
+          <t/>
         </is>
       </c>
       <c r="J80" t="e">
@@ -5386,7 +5386,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t/>
+          <t>fetcroja</t>
         </is>
       </c>
       <c r="J82" t="e">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>anhydrouscefixime,cefixim,cefixima,cefiximeanhydrous,cefiximehydrate,cefiximum,cefixoral,cefspan,cephoral,citropen,denvar,necopen,oroken,suprax,tricef,unixime</t>
+          <t>cefixim,cefixima,cefiximum,cefixoral,cefspan,cephoral,citropen,denvar,necopen,oraken,oroken,suprax,tricef,unixime</t>
         </is>
       </c>
       <c r="J83">
@@ -5576,7 +5576,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>bestron,cefmax,cefmenoxima,cefmenoximum</t>
+          <t>bestron,cefmenoxima,cefmenoximum,tacef</t>
         </is>
       </c>
       <c r="J85" t="e">
@@ -5640,7 +5640,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>cefmetazolesodium,cefmetazolo,cefmetazolum</t>
+          <t>cefmetazol,cefmetazolo,cefmetazolum,cefmetazon,metafar,zefazone</t>
         </is>
       </c>
       <c r="J86" t="e">
@@ -5700,7 +5700,7 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>cefminoxum</t>
+          <t>alteporina,cefminoxhydrate,cefminoxum,meicelin,tencef</t>
         </is>
       </c>
       <c r="J87" t="e">
@@ -5764,7 +5764,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>cefodizima,cefodizimeacid,cefodizimedisodium,cefodizimum,cefodizme,diezime,modivid,neucef,timecef</t>
+          <t>cefodizima,cefodizimum,cefodizme,diezime,kenicef,modivid,neucef,timecef</t>
         </is>
       </c>
       <c r="J88" t="e">
@@ -5828,7 +5828,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>cefonicido,cefonicidum,monocef</t>
+          <t>cefonicide,cefonicido,cefonicidsalt,cefonicidum,monocef,monocid</t>
         </is>
       </c>
       <c r="J89" t="e">
@@ -5892,7 +5892,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>bioperazone,cefobid,cefoperazine,cefoperazon,cefoperazoneacid,cefoperazono,cefoperazonum,cefozon,medocef,myticef,pathozone,peracef</t>
+          <t>bioperazone,cefob,cefobid,cefobis,cefoneg,cefoper,cefoperazin,cefoperazine,cefoperazon,cefoperazona,cefoperazonesalt,cefoperazono,cefoperazonum,cefozon,medocef,myticef,pathozone,peracef,tomabef</t>
         </is>
       </c>
       <c r="J90" t="e">
@@ -6020,7 +6020,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>ceforanido,ceforanidum,precef,radacef</t>
+          <t>ceforanido,ceforanidum,precef</t>
         </is>
       </c>
       <c r="J92" t="e">
@@ -6080,7 +6080,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>cefoselissulfate,wincef,winsef</t>
+          <t>winsef</t>
         </is>
       </c>
       <c r="J93" t="e">
@@ -6142,7 +6142,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>cefotaxim,cefotaxima,cefotaximaacid,cefotaximeacid,cefotaximhikma,cefotaximum,cephotaxime,claforan,omnatax</t>
+          <t>anticefotaxime,cefotax,cefotaxim,cefotaxima,cefotaximesalt,cefotaximsalt,cefotaximum,cephotaxim,cephotaxime,claforan,kefotex,omnatax,pretor,ralopar,taxim,tolycar,tolycor,zariviz</t>
         </is>
       </c>
       <c r="J94" t="e">
@@ -6380,7 +6380,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>apacef,cefotan,cefotetanacid,cefotetanfreeacid,cefotetanum</t>
+          <t>apacef,apatef,cefotetanum</t>
         </is>
       </c>
       <c r="J98" t="e">
@@ -6444,7 +6444,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>cefotiamum,ceradolan,ceradon,haloapor</t>
+          <t>aspil,cefotiamum,ceradon,halospor,pansporin,pansporine,spizef</t>
         </is>
       </c>
       <c r="J99">
@@ -6506,7 +6506,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>cefotiamcilexetil,pansporint</t>
+          <t>taketiam,texodil</t>
         </is>
       </c>
       <c r="J100" t="e">
@@ -6564,7 +6564,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t/>
+          <t>cefovecinsalt,convenia</t>
         </is>
       </c>
       <c r="J101" t="e">
@@ -6626,7 +6626,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>cefoxitina,cefoxitine,cefoxitinum,cefoxotin,cenomycin,cephoxitin,mefoxin,mefoxitin,rephoxitin</t>
+          <t>betacef,cefoxil,cefoxitina,cefoxitine,cefoxitinsalt,cefoxitinum,cefoxotin,cenomycin,farmoxin,mefoxin,mefoxithin,mefoxitin,merxin,rephoxitin</t>
         </is>
       </c>
       <c r="J102" t="e">
@@ -6744,7 +6744,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t/>
+          <t>firstcin,imidazo</t>
         </is>
       </c>
       <c r="J104" t="e">
@@ -6804,7 +6804,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>cefpimizol,cefpimizolesodium,cefpimizolum</t>
+          <t>ajicef,cefpimizol,cefpimizolesalt,cefpimizolum,renilan</t>
         </is>
       </c>
       <c r="J105" t="e">
@@ -6866,7 +6866,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>cefpiramideacid,cefpiramido,cefpiramidum</t>
+          <t>cefpiramida,cefpiramidesalt,cefpiramido,cefpiramidum,sepatren,suncefal,tamicin</t>
         </is>
       </c>
       <c r="J106" t="e">
@@ -6930,7 +6930,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>broact,cefpiroma,cefpiromum,cefrom,cerfpirome,keiten</t>
+          <t>broact,cefir,cefpiroma,cefpiromum,cefrom,keiten,romecef</t>
         </is>
       </c>
       <c r="J107" t="e">
@@ -6994,7 +6994,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>cefpodoxima,cefpodoximacid,cefpodoximeacid,cefpodoximum,epoxim</t>
+          <t>cefpodoxima,cefpodoximum,epoxim</t>
         </is>
       </c>
       <c r="J108">
@@ -7054,7 +7054,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>cefodox,cefoprox,cefpodoximeproxetil,cepodem,orelox,oreloxpaed,otreon,podomexef,simplicef,vantin</t>
+          <t>banan,cefodox,cefoprox,cefpoderm,cefpodoximproxetil,cepodem,doxef,orelox,otreon,podomexef,simplicef,vantin</t>
         </is>
       </c>
       <c r="J109" t="e">
@@ -7174,7 +7174,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>arzimol,brisoral,cefprozilanhydrous,cefprozilhydrate,cefprozilo,cefprozilum,cefzil,cronocef,procef,serozil</t>
+          <t>arzimol,brisoral,cefprozilo,cefprozilum,cronocef,procef,serozil</t>
         </is>
       </c>
       <c r="J111">
@@ -7234,7 +7234,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>cefquinoma,cefquinomum,cobactan</t>
+          <t>cefquinoma,cefquinomum,cobactan,quinolinium</t>
         </is>
       </c>
       <c r="J112" t="e">
@@ -7360,7 +7360,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>cefonomil,cefsulodine,cefsulodino,cefsulodinum</t>
+          <t>cefomonil,cefonomil,cefsulodine,cefsulodinhydrate,cefsulodino,cefsulodinum,pseudocef,pseudomonil,pyocefal,sulcephalosporin,takesulin,tilmapor,ulfaret</t>
         </is>
       </c>
       <c r="J114" t="e">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>ceftarolinefosamil,teflaro,zinforo</t>
+          <t>ceftaroine,teflaro,zinforo</t>
         </is>
       </c>
       <c r="J116" t="e">
@@ -7600,7 +7600,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>ceftazidim,ceftazidima,ceftazidimum,ceptaz,fortaz,fortum,pentacef,tazicef,tazidime</t>
+          <t>ceftazimide,ceptaz,fortam,fortaz,fortum,glazidim,kefazim,modacin,pentacef,tazicef,tazidime,tizime,zidim</t>
         </is>
       </c>
       <c r="J118" t="e">
@@ -7904,7 +7904,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>ceftezol,ceftezolo,ceftezolum,demethylcefazolin</t>
+          <t>alomen,ceftezol,ceftezolesalt,ceftezolo,ceftezolum,celoslin,demethylcefazolin,falomesin</t>
         </is>
       </c>
       <c r="J123" t="e">
@@ -7968,7 +7968,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>ceftem,ceftibutendihydrate,ceftibutene,ceftibutenhydrate,ceftibuteno,ceftibutenum,ceftibutin,cephem,ceprifran,isocef,keimax</t>
+          <t>cedax,ceftem,ceftibutene,ceftibuteno,ceftibutenum,ceftibutin,ceprifran,isocef,keimax,seftem</t>
         </is>
       </c>
       <c r="J124">
@@ -8028,7 +8028,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>ceftiofurum,excede,excenel,naxcel</t>
+          <t>ceftiofurum,excenel,naxcel</t>
         </is>
       </c>
       <c r="J125" t="e">
@@ -8090,7 +8090,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>cefizox,ceftisomin,ceftix,ceftizoxima,ceftizoximum,epocelin,eposerin</t>
+          <t>cefizox,ceftix,ceftizoxima,ceftizoximesalt,ceftizoximum,eposerin</t>
         </is>
       </c>
       <c r="J126" t="e">
@@ -8270,7 +8270,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t/>
+          <t>zevtera</t>
         </is>
       </c>
       <c r="J129" t="e">
@@ -8398,7 +8398,7 @@
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>biotrakson,cefatriaxone,cefatriaxonehydrate,ceftriaxon,ceftriaxona,ceftriaxonesodium,ceftriaxonum,ceftriazone,cephtriaxone,longacef,rocefin,rocephalin,rocephin,rocephine,rophex</t>
+          <t>biotrakson,ceftriaxon,ceftriaxona,ceftriaxonum,ceftriazone,rocefin,rocephalin,rocephin,rocephine,rophex</t>
         </is>
       </c>
       <c r="J131" t="e">
@@ -8526,7 +8526,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>biofuroksym,cefuril,cefuroxim,cefuroxima,cefuroximeacid,cefuroximine,cefuroximo,cefuroximum,cephuroxime,kefurox,sharox,zinacef,zinacefdanmark</t>
+          <t>anaptivan,biociclin,biofuroksym,bioxima,cefofix,cefumax,cefurex,cefuril,cefurox,cefuroxim,cefuroxima,cefuroximesalt,cefuroximine,cefuroximo,cefuroximum,cephuroxime,cetroxil,colifossim,curoxim,curoxima,curoxime,froxal,furoxil,kefurox,kesint,ketocef,lifurox,medoxim,sharox,spectrazolr,ultroxim,zinacef,zinnat</t>
         </is>
       </c>
       <c r="J133">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>altacef,bioracef,cefaks,cefazine,ceftin,cefurax,cefuroximaxetil,cefuroximeaxetil,celocid,cepazine,cethixim,cetoxil,coliofossim,elobact,forcef,furoxime,kalcef,maxitil,medoxm,nivador,novador,novocef,oraxim,zinnat</t>
+          <t>bioracef,ceftin,cefurax,cefuroximaxetil,celocid,cepazine,cethixim,cetoxil,coliofossim,curocef,elobact,furoxime,kalcef,maxitil,medoxm,nivador,novador,novocef,oraxim,zinat,zoref</t>
         </is>
       </c>
       <c r="J134" t="e">
@@ -8708,7 +8708,7 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>cefuzoname,cefuzonamsodium,cefuzonamum</t>
+          <t>cefuzoname,cefuzonamum,cefzoname,cosmosin</t>
         </is>
       </c>
       <c r="J136" t="e">
@@ -8770,7 +8770,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>anspor,cefradin,cefradina,cefradine,cefradinehydrate,cefradinum,cekodin,cephradin,cephradineanhydrous,cephradinehydrate,eskacef,infexin,megacef,sefril,velocef,velosef</t>
+          <t>anspor,cefradin,cefradina,cefradine,cefradinum,cekodin,cephradin,ecosporina,eskacef,infexin,megacef,sefril,velocef,velosef</t>
         </is>
       </c>
       <c r="J137">
@@ -8894,7 +8894,7 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>alficetyn,ambofen,amphenicol,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,chemiceticol,chemicetin,chemicetina,chlomin,chlomycol,chloramex,chloramfenikol,chloramficin,chloramfilin,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlormycetinr,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocide,chlorocidinc,chlorocidinctetran,chlorocids,chlorocin,chlorocol,chlorofair,chlorojectl,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chloropticsop,chlorovules,chlorsig,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramical,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,cloromissan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextromycetin,doctamicina,duphenicol,econochlor,embacetin,emetren,enicol,enteromycetin,erbaplast,ertilen,farmicetina,fenicol,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,interomycetine,intramycetin,intramyctin,isicetin,ismicetina,isophenicol,isoptofenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,klorocids,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromicetina,loromisan,loromisin,mastiphen,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,myscel,normimycinv,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,quemicetina,rivomycin,romphenil,ronfenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,sintomicetiner,snophenicol,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,viceton</t>
+          <t>alficetyn,ambofen,amphenicol,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,chemicetin,chemicetina,chlomin,chlomycol,chloramex,chloramfenikol,chloramficin,chloramfilin,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocide,chlorocin,chlorocol,chlorofair,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chlorovules,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextramycin,dextromycetin,doctamicina,econochlor,embacetin,emetren,enicol,enteromycetin,erbaplast,ertilen,farmicetina,fenicol,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,intramycetin,isicetin,ismicetina,isophenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromisan,loromisin,mastiphen,maybridge,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,petnamycetin,quemicetina,rivomycin,romphenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,viceton</t>
         </is>
       </c>
       <c r="J139">
@@ -8960,7 +8960,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>acronize,aueromycin,aureocina,aureomycin,aureomykoin,biomitsin,biomycin,biomycina,chlormax,chlorotetracycline,chlortetracyclinum,chrysomykine,clortetraciclina,duomycin,flamycin,uromycin</t>
+          <t>acronize,alexomycin,aueromycin,aureocarmyl,aureociclina,aureocina,aureocycline,aureomycin,aureomykoin,aurofac,auxeomycin,biomitsin,biomycin,chlormax,chlorotetracycline,chlortetracyclinum,chrysomykine,clorocipan,clortetraciclina,clortetrin,declomycin,declostatin,deganol,demeclor,demeplus,demetraciclina,demetraclin,detracin,detravis,diuciclin,duomycin,elkamicina,flamycin,isphamycin,ledermicina,ledermycin,ledermycine,mexocine,novotriclina,pennchlor,perciclina,periciclina,sumaclina,tetra,uromycin,veraciclina</t>
         </is>
       </c>
       <c r="J140">
@@ -9082,7 +9082,7 @@
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>butaconazole,butoconazol,butoconazolum,ciclodan,ciclopiroxgel,ciclopiroxolamin,ciclopiroxum,compositenstarke,dahlin,femstat,gynofort,loprox,loproxcream,loproxgel,penlac,polyfructosanum,stieprox</t>
+          <t/>
         </is>
       </c>
       <c r="J142" t="e">
@@ -9144,7 +9144,7 @@
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>azolinicacid,cinobac,cinobactin,cinoxacine,cinoxacino,cinoxacinum,clinoxacin,noxigram,uronorm</t>
+          <t>cinobac,cinobactin,cinoxacine,cinoxacino,cinoxacinum,clinoxacin,noxigram,uronorm</t>
         </is>
       </c>
       <c r="J143">
@@ -9208,7 +9208,7 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>alconcilox,auripro,bacquinor,baflox,baycip,bernoflox,cetraxal,ciflox,cifloxin,ciloxan,ciplus,ciprecu,ciprine,ciprinol,ciprobay,ciprobayuro,ciprocinol,ciprodar,ciproflox,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprogis,ciproiv,ciprolin,ciprolon,cipromycin,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciproxl,ciproxr,ciriax,citopcin,corsacin,cyprobay,fimoflox,flociprin,ipiflox,italnik,linhaliq,otiprio,probiox,proflaxin,quinolid,quintor,rancif,roxytal,septicide,sophixinofteno,spitacin,superocin,velmonit,velomonit,zumaflox</t>
+          <t>alcipro,bacquinor,baflox,belmacina,bernoflox,catex,cenin,ceprimax,cetraxal,ciflan,ciflosin,ciflox,cifloxin,cilab,cilox,ciloxan,cipad,ciplus,ciprecu,ciprenit,ciprine,ciprinol,cipro,ciprobay,ciprocinal,ciprocinol,ciprodar,ciproflox,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprofur,ciprogis,ciproktan,ciprolin,ciprolon,cipromycin,cipronex,ciprooxacin,cipropol,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciriax,citeral,citopcin,cixan,corsacin,cunesin,cycin,cyprobay,cyproxan,disfabac,felixene,fimoflox,flociprin,floxacipron,flunas,globuce,inkamil,ipiflox,italnik,keefloxin,linhaliq,loxacid,loxan,lypro,megaflox,microgan,nixin,novidat,novoquin,ofitin,oftacilox,ophaflox,otiprio,phaproxin,piprol,plenolyt,probiox,proflaxin,proksi,proquin,proxacin,quinoflox,quinolid,quintor,quipro,rancif,renator,roflazin,roxytal,sepcen,septicide,septocipro,siprogut,sophixin,spitacin,strox,suiflox,superocin,supraflox,uritent,utiminx,velmonit,zumaflox</t>
         </is>
       </c>
       <c r="J144">
@@ -9460,7 +9460,7 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>abbotic,astromen,biaxin,biaxinfilmtab,biaxinhp,biaxinxl,biaxinxlfilmtab,bicrolid,clacee,clacid,clacine,clambiotic,clarem,claribid,claricide,claridar,claripen,clarith,clarithromycine,clarithromycinum,claritromicina,clathromycin,crixan,cyllid,cyllind,fromilid,heliclar,klabax,klacid,klaciped,klaricid,klaricidhp,klaricidpediatric,klaricidxl,klarid,klarin,kofron,mabicrol,macladin,maclar,prevpac,veclam,vikrol,zeclar</t>
+          <t>abbotic,abboticine,astromen,biaxin,bicrolid,bristamycin,clacee,clacid,clacine,clambiotic,clarem,claribid,claricide,claridar,claripen,clarith,clarithromycine,clarithromycinum,claritromicina,clarosip,clathromycin,crixan,cyllid,cyllind,eratrex,esinol,ethril,fromilid,gallimycin,helas,heliclar,klabax,klacid,klaciped,klaricid,klarid,klarin,kofron,mabicrol,macladin,maclar,mavid,meberyt,pediamycin,qidmycin,veclam,wyamycin,zeclar</t>
         </is>
       </c>
       <c r="J148">
@@ -9522,7 +9522,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>acideclavulanique,acidoclavulanico,acidumclavulanicum,clavulanate,clavulanateacid,clavulanatelithium,clavulanicacid,clavulansaeure,clavulansaure,clavulinicacid,clavulox,serdaxin,sodiumclavulanate</t>
+          <t>amonate,clavulanate,clavulanateacid,clavulansaeure,clavulansaure,clavulox,serdaxin</t>
         </is>
       </c>
       <c r="J149" t="e">
@@ -9642,7 +9642,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>antirobe,chlolincocin,clindaderm,clindamicina,clindamycine,clindamycinum,clinimycin,dalacinc,dalacine,klimicin,sobelin</t>
+          <t>antirobe,chlolincocin,chlorlincocin,cleocin,clindamicina,clindamycine,clindamycinum,clinimycin,clinsol,clintabs,dalacine,klimicin,klindan,sobelin</t>
         </is>
       </c>
       <c r="J151">
@@ -9766,7 +9766,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>chlofazimine,clofazimin,clofazimina,clofaziminum,colfazimine,lampren,lamprene,riminophenazine</t>
+          <t>chlofazimine,clofazimina,clofaziminum,colfazimine,lampren,lamprene,phenazine,riminophenazine</t>
         </is>
       </c>
       <c r="J153">
@@ -9830,7 +9830,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>clofoctolo,clofoctolum,gramplus,octofene</t>
+          <t>clofoctolo,clofoctolum,gramplus,octofene,phenol</t>
         </is>
       </c>
       <c r="J154" t="e">
@@ -9892,7 +9892,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>chlomethocillin,clometacillin,clometocilina,clometocilline,clometocillinum,rixapen</t>
+          <t>chlomethocillin,clometacillin,clomethacillin,clomethocillin,clometocilina,clometocilline,clometocillinsalt,clometocillinum,penicilline,rixapen</t>
         </is>
       </c>
       <c r="J155">
@@ -9956,7 +9956,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>chlormethylencycline,clomociclina,clomocyclin,clomocyclinum,megaclor</t>
+          <t>clomociclina,clomocyclinum,megaclor</t>
         </is>
       </c>
       <c r="J156">
@@ -10016,7 +10016,7 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>canesten,canestencream,canestene,canestensolution,canestine,canifug,chlotrimazole,cimitidine,clomatin,clotrimaderm,clotrimadermcream,clotrimazol,clotrimazolum,cutistad,desamixf,diphenylmethane,empecid,esparol,femcare,gynelotrimin,jidesheng,kanesten,klotrimazole,lotrimax,lotrimin,lotriminaf,lotriminafcream,lotriminaflotion,lotriminafsolution,lotrimincream,lotriminlotion,lotriminsolution,monobaycuten,mycelax,mycelex,mycelexcream,mycelexg,mycelexotc,mycelexsolution,mycelextroches,mycelextwinpack,myclocream,myclosolution,myclospraysolution,mycofug,mycosporin,mykosporin,nalbix,otomax,pedisafe,rimazole,stiemazol,tibatin,trimysten,trivagizole,veltrim</t>
+          <t>alevazol,bisphenyl,canesten,canestene,canestine,canifug,chlotrimazole,clomatin,clotrimaderm,clotrimazol,clotrimazolum,coltrimazole,cutistad,diphenylmethane,empecid,esparol,femmesil,footlogix,fortinia,gynix,imidazole,jidesheng,klotrimazole,lakesia,lombazol,lombazole,lombazolum,lotrimax,lotrimin,monobaycuten,mycelax,mycelex,mycofug,mycosporin,mykosporin,nalbix,otomax,pedesil,pedisafe,rimazole,ringworm,stiemazol,tibatin,trimysten,trivagizole</t>
         </is>
       </c>
       <c r="J157" t="e">
@@ -10078,7 +10078,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>chloroxacillin,clossacillina,cloxacilina,cloxacilline,cloxacillinna,cloxacillinsodium,cloxacillinum,cloxapen,methocillins,orbenin,syntarpen,tegopen</t>
+          <t>ankerbin,austrastaph,biocloxin,brispen,chloroxacillin,ciclex,clocil,clossacillina,cloxacilina,cloxacillinanhydrous,cloxacilline,cloxacillinsalt,cloxacillinum,cloxapen,constaphyl,dariclox,dichlorstapenor,diclocil,dicloxacillinhydrate,diflor,digloxilline,dycill,dynapen,ekvacillin,gelstaph,novapen,noxaben,orbenin,pathocil,stampen,staphybiotic,syntarpen,syntarpensalt,tegopen</t>
         </is>
       </c>
       <c r="J158">
@@ -10144,7 +10144,7 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>belcomycine,colimycin,colimycinsulphate,colisticin,colistimethate,colistimethatesodium,colistinsulfate,colistinsulphate,colobreathe,colomycin,colymycin,polymyxine,polymyxinesulfate,promixin,totazina</t>
+          <t>colimycin,colisticin,colisticina,colistina,colistine,colistinum,colobreathe,colomycin,kangdisu,kolimitsin,kolimycin,promixin,sogecoli,totazina</t>
         </is>
       </c>
       <c r="J159">
@@ -10268,7 +10268,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>cicloserina,closerin,closina,cyclorin,cycloserin,cycloserinum,farmiserina,micoserina,miroserina,miroseryn,novoserin,oxamicina,oxamycin,seromycin,tebemicina,tisomycin,wasserina</t>
+          <t>cicloserina,closerin,closina,cyclorin,cycloserin,cycloserinum,farmiserina,levcicloserina,levcycloserine,levcycloserinum,micoserina,miroserina,miroseryn,novoserin,oxamicina,oxamycin,seromycin,tebemicina,tisomycin,wasserina</t>
         </is>
       </c>
       <c r="J161">
@@ -10332,7 +10332,7 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>dalvance</t>
+          <t>dalbavancina,dalvance,xydalba,zeven</t>
         </is>
       </c>
       <c r="J162" t="e">
@@ -10454,7 +10454,7 @@
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>aczone,aralditeht,atrisone,avlosulfon,avlosulfone,avlosulphone,avsulfor,bissulfone,bissulphone,croysulfone,croysulphone,dapson,dapsona,dapsonum,diaphenylsulfon,diaphenylsulfone,diaphenylsulphon,diaphenylsulphone,dimitone,diphenasone,diphone,disulfone,disulone,disulphone,dubronax,dubronaz,dumitone,eporal,metabolitec,novophone,protogen,servidapson,slphadione,sulfadione,sulfona,sulfoneucb,sulfonyldianiline,sulphadione,sulphonyldianiline,sumicures,tarimyl,udolac</t>
+          <t>aczone,atrisone,avlosulfon,avlosulfone,avlosulphone,benzenamide,benzenamine,bissulfone,bissulphone,croysulfone,croysulphone,dapson,dapsona,dapsonum,daspone,diaphenylsulfon,diaphenylsulfone,diaphenylsulphon,diaphenylsulphone,diphenasone,diphone,disulfone,disulone,disulphone,dubronax,dumitone,eporal,medapsol,novophone,servidapson,sulfadione,sulfona,sulfonyldianiline,sulphadione,sulphonyldianiline,tarimyl,udolac,undolac</t>
         </is>
       </c>
       <c r="J164">
@@ -10518,7 +10518,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>cidecin,cubicin,dapcin,daptomicina,daptomycine,daptomycinum</t>
+          <t>cidecin,cubicin,dapcin,daptomicina,daptomycine,daptomycinum,deptomycin</t>
         </is>
       </c>
       <c r="J165" t="e">
@@ -10708,7 +10708,7 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>bioterciclin,clortetrin,declomycin,deganol,demeclociclina,demeclocyclinum,demeclor,demetraclin,diuciclin,elkamicina,ledermycin,mexocine,novotriclina,perciclina,sumaclina</t>
+          <t>demeclociclina,demeclocyclinum</t>
         </is>
       </c>
       <c r="J168">
@@ -10772,7 +10772,7 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>debecacin,dibekacina,dibekacine,dibekacinsulfate,dibekacinum,dideoxykanamycinb,kappati,orbicin,panamicin</t>
+          <t>debecacin,dibekacina,dibekacine,dibekacinum,kappati,panamicin</t>
         </is>
       </c>
       <c r="J169" t="e">
@@ -10836,7 +10836,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>dichloroxacillin,diclossacillina,dicloxaciclin,dicloxacilin,dicloxacilina,dicloxacillina,dicloxacilline,dicloxacillinsodium,dicloxacillinum,dicloxacycline,dycill,dynapen,maclicine,nmdicloxacillin,pathocil</t>
+          <t>dichloroxacillin,diclossacillina,dicloxaciclin,dicloxacilin,dicloxacilina,dicloxacillina,dicloxacilline,dicloxacillinum,dicloxacycline,maclicine</t>
         </is>
       </c>
       <c r="J170">
@@ -10898,7 +10898,7 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>dicural,pulsaflox</t>
+          <t>dicural,difloxacine,pulsaflox</t>
         </is>
       </c>
       <c r="J171" t="e">
@@ -11024,7 +11024,7 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>doribax,doripenemhydrate,finibax</t>
+          <t>doribax,dripenem,finibax</t>
         </is>
       </c>
       <c r="J173" t="e">
@@ -11088,7 +11088,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>atridox,azudoxat,deoxymykoin,dossiciclina,doxcyclineanhydrous,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycyclinecalcium,doxycyclinehyclate,doxycyclinum,doxylin,doxysol,doxytec,doxytetracycline,hydramycin,investin,jenacyclin,liviatin,monodox,oracea,periostat,ronaxan,spanor,supracyclin,vibramycin,vibramycine,vibramycinnovum,vibravenos,zenavod</t>
+          <t>abbocin,alamycin,aquacycline,biosolvomycin,biotet,bisolvomycin,chrysocin,dalimycin,dalinmycin,deoxymykoin,dossiciclina,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycyclinum,doxylin,doxysol,doxytetracycline,elinton,engemycin,hydrocyclin,imperacin,intaloxin,investin,jenacyclin,liquachel,liviatin,macodyn,mepatar,microdox,mondoxyne,monodox,morgidox,ocudox,okebo,oracea,otetryn,oxacycline,oxamycen,oxatet,oxlopar,oxybiocycline,oxycycline,oxydon,oxyject,oxymykoin,oxysteclin,oxytet,oxytetral,oxytetrin,oxytracyl,oxyvet,stecsolin,supracyclin,terraject,terramycin,toxinal,unimycin,vendarcin,vibramycin,vibramycine,vivox,zenavod</t>
         </is>
       </c>
       <c r="J174">
@@ -11154,7 +11154,7 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>econazol,econazolum,ecostatin,ecostatincream,palavale,pevaryl,spectazole,spectazolecream</t>
+          <t>bromazil,chloramizol,clinafarm,deccosil,deccozil,econazol,econazolum,ecostatin,ekonazole,enilconazol,enilconazole,eniloconazol,fecundal,florasan,freshgard,freshguard,fungaflor,fungazil,imaverol,imaversol,imazalil,magnate,spectazole</t>
         </is>
       </c>
       <c r="J175" t="e">
@@ -11274,7 +11274,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>almitil,bactidan,bactidron,comprecin,enofloxacine,enoksetin,enoram,enoxacina,enoxacine,enoxacino,enoxacinum,enoxen,enoxin,enoxor,flumark,penetrex</t>
+          <t>abenox,almitil,bactidan,bactidron,comprecin,enofloxacine,enoksetin,enoram,enoxacina,enoxacine,enoxacino,enoxacinum,enoxen,enoxin,enoxor,flumark,penetrex</t>
         </is>
       </c>
       <c r="J177">
@@ -11334,7 +11334,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>baytril,enrofloxacine,enrofloxacino,enrofloxacinum,enroxil</t>
+          <t>baytril,enroflox,enrofloxacine,enrofloxacino,enrofloxacinum,enroquin,enrosite,enroxil,quellaxcin,tenotryl,zobuxa</t>
         </is>
       </c>
       <c r="J178" t="e">
@@ -11392,7 +11392,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>enviomicina,enviomycina,enviomycinum,tuberactin</t>
+          <t>enviomicina,enviomycina,enviomycine,enviomycinum,tuberactin</t>
         </is>
       </c>
       <c r="J179" t="e">
@@ -11514,7 +11514,7 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>dexacillin,dihydroampicillin,epicilina,epicilline,epicillinum</t>
+          <t>dexacillin,dihydroampicillin,epicilina,epicilline,epicillinum,spectacillin</t>
         </is>
       </c>
       <c r="J181">
@@ -11702,7 +11702,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>invanz</t>
+          <t>ertapenemsalt,invanz</t>
         </is>
       </c>
       <c r="J184" t="e">
@@ -11766,7 +11766,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>abboticin,abomacetin,acneryne,acnesol,aknecordeslosung,aknedermerygel,aknemycin,austrias,benzamycin,bristamycin,derimer,deripil,dotycin,dumotrycin,emuvin,emycin,endoeritrin,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,erycen,erycette,erycin,erycinum,erycsprinkles,eryderm,erydermer,erygel,eryhexal,erymax,erymed,erypar,erysafe,erytab,erythrocin,erythrocinstearate,erythroderm,erythrogran,erythroguent,erythromid,erythromycina,erythromycinbase,erythromycine,erythromycines,erythromycinlactate,erythromycinum,erytop,erytrociclin,ilocaps,ilosone,iloticina,ilotycin,ilotycingluceptate,ilotycints,inderm,indermgel,indermretcin,latotryd,lederpax,mephamycin,mercina,oftamolets,paediathrocin,pantoderm,pantodrin,pantomicina,pcedispertab,pharyngocin,primacine,propiocine,proterytrin,retcin,robimycin,romycin,sansac,skidgele,staticin,stiemicyn,stiemycin,theramycinz,tiloryth,tiprocin,torlamicina,udimaerygel,wyamycins</t>
+          <t>abboticin,abomacetin,acneryne,acnesol,aknemycin,aknin,benzamycin,derimer,deripil,dotycin,dumotrycin,emgel,emuvin,emycin,endoeritrin,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,erycen,erycette,erycin,erycinum,eryderm,erydermer,erygel,eryhexal,erymax,erymed,erysafe,erytab,erythro,erythroderm,erythrogran,erythroguent,erythromast,erythromid,erythromycine,erythromycinum,erytop,erytrociclin,ilocaps,ilosone,iloticina,ilotycin,inderm,latotryd,lederpax,mephamycin,mercina,oftamolets,pantoderm,pantodrin,pantomicina,pharyngocin,primacine,propiocine,proterytrin,retcin,robimycin,romycin,sansac,spotex,staticin,stiemicyn,stiemycin,tiprocin,torlamicina,wemid</t>
         </is>
       </c>
       <c r="J185">
@@ -11832,7 +11832,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>aethambutolum,diambutol,ebutol,etambutol,etambutolo,etapiam,ethambutolum,myambutol,mycobutol,purderal,servambutol,tibutol</t>
+          <t>aethambutolum,dadibutol,diambutol,etambutol,etambutolo,ethambutolum,myambutol,purderal,servambutol,tibutol</t>
         </is>
       </c>
       <c r="J186">
@@ -11960,7 +11960,7 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>aethionamidum,aetina,aetiva,amidazin,amidazine,ethatyl,ethimide,ethina,ethinamide,ethionamidum,ethioniamide,ethylisothiamide,ethyonomide,etimid,etiocidan,etionamid,etionamida,etionamide,etioniamid,etionid,etionizin,etionizina,etionizine,fatoliamid,iridocin,iridocinbayer,iridozin,isothin,isotiamida,itiocide,nicotion,nisotin,nizotin,rigenicid,sertinon,teberus,thianid,thianide,thioamide,thiodine,thiomid,thioniden,tianid,tiomid,trecator,trecatorsc,trekator,trescatyl,trescazide,tubenamide,tubermin,tuberoid,tuberoson</t>
+          <t>aethionamidum,aetina,aetiva,amidazin,amidazine,atina,ethimide,ethina,ethinamide,ethionamidum,ethioniamide,ethylisothiamide,ethyonomide,etimid,etiocidan,etionamid,etionamida,etionamide,etioniamid,etionid,etionizin,etionizina,etionizine,fatoliamid,iridocin,iridozin,isothin,isotiamida,itiocide,nicotion,nisotin,nizotin,rigenicid,sertinon,teberus,thianid,thianide,thioamide,thiodine,thiomid,thioniden,tianid,tiomid,trecator,trekator,trescatyl,trescazide,tubenamide,tubermin,tuberoid,tuberoson</t>
         </is>
       </c>
       <c r="J188">
@@ -12020,7 +12020,7 @@
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>amprolplus,ethopabat,ethylpabate</t>
+          <t>ethopabat</t>
         </is>
       </c>
       <c r="J189" t="e">
@@ -12138,7 +12138,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>faropenemsodium,fropenem,fropenumsodium</t>
+          <t>farom,faropenemhydrate,faropenemsalt,fropenem,fropenum,furopenem</t>
         </is>
       </c>
       <c r="J191">
@@ -12198,7 +12198,7 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>dificid,dificlir,difimicin,lipiarmicin,lipiarmycin,lipiarrmycin,tiacumicinb</t>
+          <t>dificid,dificlir,difimicin,fidaxomicina,lipiarmicin,lipiarmycin,lipiarrmycin</t>
         </is>
       </c>
       <c r="J192">
@@ -12258,7 +12258,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t/>
+          <t>xtoro</t>
         </is>
       </c>
       <c r="J193" t="e">
@@ -12316,7 +12316,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>flavophospholipol,moenomycincomplex</t>
+          <t>bambermicina,bambermycine,bambermycinum,flavofosfolipol,flavophospholipol,gainpro,menomycin</t>
         </is>
       </c>
       <c r="J194" t="e">
@@ -12440,7 +12440,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>flomoxefo,flomoxefum</t>
+          <t>flomoxefo,flomoxefsalt,flomoxefum,flumarin</t>
         </is>
       </c>
       <c r="J196" t="e">
@@ -12500,7 +12500,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>aquafen,nuflor,nuflorgold</t>
+          <t>aquafen,descocin,dexawin,efnicol,fricol,hyrazin,loncor,macphenicol,masatirin,neomyson,norfenicol,nuflor,racephenicol,rincrol,thiamcol,urfamicina,urophenyl</t>
         </is>
       </c>
       <c r="J197" t="e">
@@ -12562,7 +12562,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>culpen,floxacillin,floxacillinsodium,floxapen,floxapensodiumsalt,fluclox,flucloxacilina,flucloxacilline,flucloxacillinum,fluorochloroxacillin,staphylex</t>
+          <t>bactopen,cloxacap,cloxacillinhydrate,cloxypen,floxacillin,floxacillinanhydrous,floxapen,floxapensalt,fluclomix,flucloxacilina,flucloxacilline,flucloxacillinum,flucloxin,fluorochloroxacillin,galfloxin,latocillin,orbeninhydrate,rimaflox,staphobristol,zoxin</t>
         </is>
       </c>
       <c r="J198">
@@ -12628,7 +12628,7 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>alflucoz,alfumet,alkanazole,biocanol,biozole,biozolene,canzol,cryptal,diflazon,diflucan,dimycon,elazor,flucazol,fluconazol,fluconazolecapsules,fluconazoli,fluconazolum,flucoral,flucostat,flukezol,flunazol,flunizol,flusol,fluzon,fluzone,forcan,fuconal,fungata,loitin,oxifugol,pritenzol,syscan,trican,triconal,triflucan,zoltec</t>
+          <t>alflucoz,alkanazole,baten,biocanol,biozole,biozolene,canzol,cryptal,diflazon,diflucan,dimycon,elazor,flucazol,fluconazol,fluconazoli,fluconazolum,flucoral,flucostat,flukezol,flunazol,flunizol,fluzon,forcan,fuconal,fungata,loitin,mutum,oxifugol,pritenzol,syscan,trican,triconal,triflucan,zemyc,zoltec,zonal</t>
         </is>
       </c>
       <c r="J199">
@@ -12694,7 +12694,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>alcobon,ancoban,ancobon,ancotil,ancotyl,flourocytosine,flucitosina,flucystine,flucytosin,flucytosinum,flucytosone,fluocytosine,fluorcytosine,fluorocytosine</t>
+          <t>alcobon,ancoban,ancobon,ancotil,ancotyl,flourocytosine,flucitosina,flucytosin,flucytosinum,flucytosone,fluocytosine,fluorcytosine,fluorocytosine</t>
         </is>
       </c>
       <c r="J200">
@@ -12760,7 +12760,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>apurone,fantacin,flumequino,flumequinum,flumigal,flumiquil,flumisol,flumix,imequyl</t>
+          <t>apurone,fantacin,flumequina,flumequino,flumequinum,flumigal,flumiquil,flumisol,flumix,imequyl</t>
         </is>
       </c>
       <c r="J201">
@@ -12824,7 +12824,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>flurithromicina,flurithromycime,flurithromycine,flurithromycinum,fluritromicina,fluritromycinum,flurizic</t>
+          <t>abbot,beritromicina,berythromycin,berythromycine,berythromycinum,flurithromycine,flurithromycinum,fluritromicina,fluritromycinum,flurizic,mizar</t>
         </is>
       </c>
       <c r="J202">
@@ -12884,7 +12884,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>phosfluconazole,procif,prodif</t>
+          <t>fosfluconazol,procif,prodif</t>
         </is>
       </c>
       <c r="J203" t="e">
@@ -12946,7 +12946,7 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>calciumfosfomycin,fosfocina,fosfomicin,fosfomicina,fosfomycine,fosfomycinsodium,fosfomycinum,fosfonomycin,infectophos,monuril,monurol,phosphonemycin,phosphonomycin,veramina</t>
+          <t>fosfocina,fosfomicin,fosfomicina,fosfomycine,fosfomycinum,fosfonomycin,infectophos,phosphonemycin,phosphonomycin,veramina</t>
         </is>
       </c>
       <c r="J204">
@@ -13008,7 +13008,7 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>fosmidomycina,fosmidomycine,fosmidomycinum</t>
+          <t>fosmidomicina,fosmidomycina,fosmidomycine,fosmidomycinsalt,fosmidomycinum</t>
         </is>
       </c>
       <c r="J205" t="e">
@@ -13066,7 +13066,7 @@
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>actilin,actiline,antibiotique,bycomycin,dekamyciniii,endomixin,enterfram,fradiomycin,fradiomycinb,fradiomycinum,framicetina,framidal,framycetine,framycetinsulfate,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycinb,neomycinbsulfate,neomycine,neomycinsolution,neomycinsulfate,neomycinsulphate,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycinpowderv</t>
+          <t>actilin,actiline,antibiotique,bycomycin,enterfram,fradiomycin,fradiomycinum,framicetina,framidal,framycetine,framycetinum,framycin,framygen,francetin,jernadex,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycine,neomycinum,nivemycin,soframycin,soframycine</t>
         </is>
       </c>
       <c r="J206" t="e">
@@ -13128,7 +13128,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>akritoin,furagin,furaginum,furamag,furazidine</t>
+          <t>akritoin,furagin,furaginum,furamag,furazidine,hydantoin</t>
         </is>
       </c>
       <c r="J207">
@@ -13188,7 +13188,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>bifuron,corizium,coryzium,diafuron,enterotoxon,furall,furaxon,furaxone,furazol,furazolidine,furazolidon,furazolidona,furazolidonum,furazolum,furazon,furidon,furovag,furoxaerosolpowder,furoxal,furoxane,furoxon,furoxone,furoxoneliquid,furoxoneswinemix,furozolidine,giardil,giarlam,medaron,neftin,nicolen,nifulidone,nifuran,nifurazolidone,nifurazolidonum,nitrofurazolidone,nitrofurazolidonum,nitrofuroxon,optazol,ortazol,puradin,roptazol,sclaventerol,tikofuran,topazone,trichofuron,tricofuron,tricoron,trifurox,viofuragyn</t>
+          <t>bifuron,corizium,coryzium,diafuron,enterotoxon,furall,furanzolidone,furaxon,furaxone,furazol,furazolidine,furazolidon,furazolidona,furazolidonum,furazolum,furazon,furidon,furmethoxadone,furovag,furox,furoxal,furoxane,furoxon,furoxone,furozolidine,giardil,giarlam,medaron,neftin,nicolen,nifulidone,nifuran,nifurazolidone,nifurazolidonum,nitrofuradoxon,nitrofurazolidone,nitrofurazolidonum,nitrofuroxon,optazol,ortazol,puradin,roptazol,sclaventerol,tikofuran,topazone,trichofuron,tricofuron,tricoron,trifurox,viofuragyn</t>
         </is>
       </c>
       <c r="J208" t="e">
@@ -13250,7 +13250,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>acidefusidique,acidofusidico,acidumfusidicum,flucidin,fucidate,fucidatesodium,fucidicacid,fucidin,fucidinacid,fucithalmic,fusidate,fusidateacid,fusidicacid,fusidine,fusidinicacid,ramycin,taksta</t>
+          <t>flucidin,fucidate,fucidina,fucidine,fucithalmic,fusidate,fusidicacid,fusidin,fusidine,ramycin,taksta</t>
         </is>
       </c>
       <c r="J209">
@@ -13312,7 +13312,7 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t/>
+          <t>zactran</t>
         </is>
       </c>
       <c r="J210" t="e">
@@ -13434,7 +13434,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>gatiflo,gatifloxacine,gatifloxacinhydrate,gatifloxcin,gatilox,gatiquin,gatispan,tequin,tequinandzymar,zymaxid</t>
+          <t>acorafloxacin,avarofloxacin,balofloxacin,balofox,bazucin,bilimin,bonoq,gaity,gatiflo,gatifloxacine,gatifloxcin,gatilox,gatiquin,gatispan,kinome,tequin,tymer,zymar,zymaxid,zymer</t>
         </is>
       </c>
       <c r="J212">
@@ -13500,7 +13500,7 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>factiv,factive,gemifioxacin,gemifloxacine,gemifloxacino,gemifloxacinum</t>
+          <t>factiv,gemifioxacin,gemifloxacine,gemifloxacino,gemifloxacinum</t>
         </is>
       </c>
       <c r="J213">
@@ -13566,7 +13566,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>apogen,centicin,cidomycin,garamycin,garasol,genopticliquifilm,genopticsop,gentacycol,gentafair,gentak,gentamar,gentamcinsulfate,gentamicina,gentamicine,gentamicins,gentamicinum,gentamycin,gentamycins,gentamycinum,gentavet,gentocin,jenamicin,lyramycin,oksitselanim,refobacin,refobacintm,septigen,uromycine</t>
+          <t>centicin,cidomycin,garamicin,garamycin,gentacycol,gentamicina,gentamicine,gentamicins,gentamicinum,gentamycins,gentamycinum,gentocin,lyramycin,oksitselanim,septigen,septocin</t>
         </is>
       </c>
       <c r="J214" t="e">
@@ -13684,7 +13684,7 @@
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t/>
+          <t>gepotidacina,gepotidacine</t>
         </is>
       </c>
       <c r="J216" t="e">
@@ -13746,7 +13746,7 @@
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t/>
+          <t>grepafloxacine,grepafloxacino,lungaskin,raxar,vaxar</t>
         </is>
       </c>
       <c r="J217">
@@ -13806,7 +13806,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>amudane,curlingfactor,delmofulvina,fulcin,fulcine,fulvicangrisactin,fulvicin,fulvicinbolus,fulvidex,fulvina,fulvinil,fulvistatin,fungivin,greosin,gresfeed,gricin,grifulin,grifulvin,grifulvinv,grisactin,grisactinultra,grisactinv,griscofulvin,grisefuline,griseo,griseoflulvin,griseofulvina,griseofulvine,griseofulvinforte,griseofulvinum,griseomix,griseostatin,grisetin,grisofulvin,grisovin,grisovinfp,grizeofulvin,grysio,guservin,lamoryl,likuden,likunden,murfulvin,poncyl,spirofulvin,sporostatinxan,xuanjing</t>
+          <t>amudane,delmofulvina,epigriseofulvin,fulcin,fulcine,fulvicin,fulvidex,fulvina,fulvinil,fulvistatin,fungivin,greosin,gresfeed,gricin,grifulin,grifulvin,grisactin,griscofulvin,grisefuline,griseo,griseofulviin,griseofulvina,griseofulvine,griseofulvinum,griseomix,griseostatin,grisetin,grisofulvin,grisovin,grisowen,grizeofulvin,grysio,guservin,lamoryl,likuden,likunden,murfulvin,poncyl,spiro,spirofulvin,xuanjing</t>
         </is>
       </c>
       <c r="J218">
@@ -13866,7 +13866,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>arbekacinsulfate,arbekacinsulphate,habekacinsulfate,habekacinxsulfate</t>
+          <t>amikafur,amikan,amitrex,arikayce,biklin,biodacyn,chemacin,fabianol,habekacinxsulfate,likacin,pierami</t>
         </is>
       </c>
       <c r="J219" t="e">
@@ -13990,7 +13990,7 @@
       </c>
       <c r="I221" t="inlineStr">
         <is>
-          <t>etacillina,hetacilina,hetacillinacid,hetacilline,hetacillinum,phenazacillin,versapen</t>
+          <t>etacillina,hetacilina,hetacilline,hetacillinum,natacillin,phenazacillin,versapen,versatrex</t>
         </is>
       </c>
       <c r="J221">
@@ -14050,7 +14050,7 @@
       </c>
       <c r="I222" t="inlineStr">
         <is>
-          <t>antihelmycin,hydromycinb,hygrovetine</t>
+          <t>antihelmycin,destomysin,hyanthelmix,hygromix,hygrovectine,hygrovetine</t>
         </is>
       </c>
       <c r="J222" t="e">
@@ -14166,7 +14166,7 @@
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>mersarex</t>
+          <t>iclaprime,mersarex</t>
         </is>
       </c>
       <c r="J224" t="e">
@@ -14228,7 +14228,7 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>imipemide,imipenemanhydrous,imipenemcilastatin,imipenemhydrate,imipenemum,imipenen,primaxin,recarbrio,tienamycin</t>
+          <t>imipemide,imipenemum,imipenen,primaxin,recarbrio,tienam,tienamycin</t>
         </is>
       </c>
       <c r="J225" t="e">
@@ -14406,7 +14406,7 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t/>
+          <t>benzonitrile,ravuconazole</t>
         </is>
       </c>
       <c r="J228">
@@ -14598,7 +14598,7 @@
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>abdizide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,aztisoniazid,azuren,bacillin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hidranizil,hidrasonil,hidrulta,hidrun,hycozid,hydrazid,hydrazide,hyozid,iai,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazida,isoniazide,isoniazidsa,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,lanizid,mayambutol,mybasan,neoteben,neoxin,neumandin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nydrazid,nyscozid,pelazid,percin,phthisen,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,stanozide,tebecid,tebenic,tebexin,tebilon,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
+          <t>abdizide,acetylisoniazide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,azuren,cedin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,dinocrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hidranizil,hidrasonil,hidrulta,hidrun,hycozid,hydra,hydrazid,hyozid,hyzyd,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazida,isoniazide,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,mayambutol,mybasan,neoteben,neoxin,neumandin,nevin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nitebannsc,nydrazid,nyscozid,pelazid,percin,phthisen,preparation,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,soniazid,stanozide,tebecid,tebenic,tebexin,tebilon,tebos,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisin,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,tyvid,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
         </is>
       </c>
       <c r="J231">
@@ -14726,7 +14726,7 @@
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>intraconazole,itraconazol,itraconazolo,itraconazolum,itraconzaole,itrazole,itrizole,oriconazole,sporanox</t>
+          <t>candistat,canditral,cladosal,fungitraxx,intraconazole,itrac,itraconazol,itraconazolo,itraconazolum,itraconzaole,itrafungol,itralek,itrizole,lozanoc,onmel,oriconazole,sempera,sporamelt,sporanox,sporonox,traconal,triasporin</t>
         </is>
       </c>
       <c r="J233">
@@ -14792,7 +14792,7 @@
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>jomybel,josacine,josamicina,josamycine,josamycinum</t>
+          <t>jomybel,josamicina,josamycine,josamycinum</t>
         </is>
       </c>
       <c r="J234">
@@ -14856,7 +14856,7 @@
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>kanamicina,kanamycina,kanamycinbase,kanamycine,kanamycins,kanamycinsulfate,kanamycinum,kantrex,kenamycina,klebcil,liposomalkanamycin</t>
+          <t>kanamicina,kanamycine,kanamycins,kanamycinum,kantrex,klebcil</t>
         </is>
       </c>
       <c r="J235">
@@ -15038,7 +15038,7 @@
       </c>
       <c r="I238" t="inlineStr">
         <is>
-          <t>extina,fungarest,fungoral,ketocanazole,ketoconazol,ketoconazolum,ketoderm,nizoral,xolegel</t>
+          <t>brizoral,ethanone,extina,fungarest,fungoral,ketaconazole,ketocanazole,ketoconazol,ketoconazolum,ketodan,ketoderm,ketoisdin,ketozole,kuric,levoketoconazole,nizoral,normocort,panfungol,piperazine,recorlev,sebazole,teryzolin,terzolin,tocris,xolegel</t>
         </is>
       </c>
       <c r="J238">
@@ -15098,7 +15098,7 @@
       </c>
       <c r="I239" t="inlineStr">
         <is>
-          <t>jomybel,josacine,josamicina,josamycine,josamycinum</t>
+          <t/>
         </is>
       </c>
       <c r="J239" t="e">
@@ -15156,7 +15156,7 @@
       </c>
       <c r="I240" t="inlineStr">
         <is>
-          <t>avatec,lasalocida,lasalocide,lasalocidea,lasalocido,lasalocidum</t>
+          <t>avatec,bovate,bovatec,lasalocide,lasalocido,lasalocidsalt,lasalocidum</t>
         </is>
       </c>
       <c r="J240" t="e">
@@ -15218,7 +15218,7 @@
       </c>
       <c r="I241" t="inlineStr">
         <is>
-          <t/>
+          <t>lasvic</t>
         </is>
       </c>
       <c r="J241">
@@ -15282,7 +15282,7 @@
       </c>
       <c r="I242" t="inlineStr">
         <is>
-          <t>disodiummoxalactam,festamoxin,lamoxactam,latamoxefum,moxalactamsupplement,shiomarin</t>
+          <t>dilatamoxef,festamoxin,lamoxactam,latamoxefum,morrhuate,moxalactamsalt,moxam,shiomarin</t>
         </is>
       </c>
       <c r="J242" t="e">
@@ -15342,7 +15342,7 @@
       </c>
       <c r="I243" t="inlineStr">
         <is>
-          <t>xenleta</t>
+          <t>lefamulinacetate,xenleta</t>
         </is>
       </c>
       <c r="J243" t="e">
@@ -15400,7 +15400,7 @@
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>lenampicilina,lenampicilline,lenampicillinhcl,lenampicillinum</t>
+          <t>lenampicilina,lenampicilline,lenampicillinum,takacillin,valacillin,varacillin</t>
         </is>
       </c>
       <c r="J244" t="e">
@@ -15462,7 +15462,7 @@
       </c>
       <c r="I245" t="inlineStr">
         <is>
-          <t>aeroquin,anhydrousofloxacin,cravit,cravithydrate,cravitiv,cravitophthalmic,elequine,floxacin,floxel,fluoroquinolone,iquixhydrate,leroxacin,lesacin,levaquin,levaquinhydrate,levofiexacin,levofloxacine,levofloxacinhydrate,levofloxacino,levofloxacinum,levokacin,levoxacin,mosardal,nofaxin,ofloxcacin,oftaquix,quinsair,quixin,reskuin,tavanic,unibiotic,venaxan,volequin</t>
+          <t>aeroquin,cravit,dextrofloxacin,dynaquin,elequine,floxacin,iquix,levaquin,levofiexacin,levofloxacine,levofloxacino,levofloxacinum,loxof,ofloxcacin,oftaquix,quinsair,quixin,tavanic,unibiotic,venaxan</t>
         </is>
       </c>
       <c r="J245">
@@ -15706,7 +15706,7 @@
       </c>
       <c r="I249" t="inlineStr">
         <is>
-          <t>bactramycin,cillimycin,frademicina,jiemycin,lincocin,lincolcina,lincolnensin,lincomicina,lincomycina,lincomycine,lincomycinum,lincorex</t>
+          <t>albiotic,bactramycin,cillimycin,frademicina,jiemycin,lincocin,lincogap,lincolcina,lincolnensin,lincomicina,lincomix,lincomycine,lincomycinum,lincomyocin,lincorex,linocin,mycivin</t>
         </is>
       </c>
       <c r="J249">
@@ -15772,7 +15772,7 @@
       </c>
       <c r="I250" t="inlineStr">
         <is>
-          <t>linezlid,linezoid,linezolide,linezolidum,zivoxid,zyvoxa,zyvoxam,zyvoxid</t>
+          <t>desfluorolinezolid,linezoid,linezolidum,zivoxid,zyvox,zyvoxa,zyvoxam,zyvoxid</t>
         </is>
       </c>
       <c r="J250">
@@ -15896,7 +15896,7 @@
       </c>
       <c r="I252" t="inlineStr">
         <is>
-          <t>lomefloxacine,lomefloxacino,lomefloxacinum,maxaquin</t>
+          <t>bareon,logiflox,lomebact,lomefloxacine,lomefloxacino,lomefloxacinum,maxaquin,maxaquine,mazaquin,okacin,okacyn,uniquin</t>
         </is>
       </c>
       <c r="J252">
@@ -15960,7 +15960,7 @@
       </c>
       <c r="I253" t="inlineStr">
         <is>
-          <t>anhydrousloracarbef,lorabid,loracabef,loracarbefum,lorbef,loribid</t>
+          <t>carbac,lorabid,loracarbefum,lorafem,lorbef,loribid</t>
         </is>
       </c>
       <c r="J253">
@@ -16024,7 +16024,7 @@
       </c>
       <c r="I254" t="inlineStr">
         <is>
-          <t>biovetin,chlortetracyclin,ciclisin,ciclolysal,ciclolysine,infaciclina,limeciclina,lisinbiotic,lymecyclin,lymecyclinum,mucomycin,ntetracycline,tetralisal,tetralysal,vebicyclysal</t>
+          <t>armyl,chlortetracyclin,ciclisin,ciclolysal,ciclolysine,eficiclina,infaciclina,limeciclina,lisinbiotic,lymecyclinum,mucomycin,ntetracycline,tetralisal,tetralysal,vebicyclysal</t>
         </is>
       </c>
       <c r="J254">
@@ -16090,7 +16090,7 @@
       </c>
       <c r="I255" t="inlineStr">
         <is>
-          <t>acidomandelico,almondacid,ammoniummandelate,amygdalicacid,benzoglycolicacid,hydroxyaceticacid,kyselinamandlova,mandelicacid,paramandelicacid,phenylglycolicacid,uromaline</t>
+          <t>amygdalate,mandelsaeure,methyl,paramandelate,phenylglycolate,phenylhydroxyacetate,uromaline</t>
         </is>
       </c>
       <c r="J255">
@@ -16208,7 +16208,7 @@
       </c>
       <c r="I257" t="inlineStr">
         <is>
-          <t>marbocyl,marbofloxacine,marbofloxacino,marbofloxacinum,zeniquin</t>
+          <t>marbocyl,marbofloxacine,marbofloxacino,marbofloxacinum,marboquin,zeniquin</t>
         </is>
       </c>
       <c r="J257" t="e">
@@ -16270,7 +16270,7 @@
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>amdinocillin,coactin,hexacillin,mecilinamo,mecillinamum,micillinam,penicillinhx,selexidin</t>
+          <t>amdinocillin,coactin,hexacillin,mecilinamo,mecillinamum,selexidin</t>
         </is>
       </c>
       <c r="J258" t="e">
@@ -16392,7 +16392,7 @@
       </c>
       <c r="I260" t="inlineStr">
         <is>
-          <t>meronem,meropen,meropenemanhydrous,meropenemhydrate,meropenemtrihydrate,meropenemum,merrem,merremiv</t>
+          <t>meronem,meropen,meropenemum,merrem</t>
         </is>
       </c>
       <c r="J260" t="e">
@@ -16514,7 +16514,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>carbavance,vabomere</t>
+          <t/>
         </is>
       </c>
       <c r="J262" t="e">
@@ -16574,7 +16574,7 @@
       </c>
       <c r="I263" t="inlineStr">
         <is>
-          <t>mesulfamido,mesulfamidum</t>
+          <t>mesulfamida,mesulfamido,mesulfamidum</t>
         </is>
       </c>
       <c r="J263" t="e">
@@ -16636,7 +16636,7 @@
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>bialatan,metaciclina,metacyclinum,methacycline,methacyclinebase,methacyclinum,methylenecycline,physiomycine,rondomycin</t>
+          <t>bialatan,metaciclina,metacyclinum,methacyclin,methacycline,methacyclinum,methylenecycline,physiomycine,rondomycin</t>
         </is>
       </c>
       <c r="J264">
@@ -16700,7 +16700,7 @@
       </c>
       <c r="I265" t="inlineStr">
         <is>
-          <t>blomopen,bonopen,celinmicina,elatocilline,fedacilinakapseln,filorex,italcinakapseln,magnipen,metabacterampullen,metambac,metampicilina,metampicillina,metampicilline,metampicillinsodium,metampicillinum,methampicillin,metiskiaampullen,micinovo,micinovoampullen,pangocilin,probiotic,rastomycink,relyothenate,ruticina,rutizina,rutizinaampullen,sedomycin,suvipen,suvipenampullen,tampilenampullen,teonicontrofen,viderpen,viderpin,vioplex</t>
+          <t>blomopen,bonopen,celinmicina,elatocilline,filorex,magnipen,metambac,metampen,metampicilina,metampicillina,metampicilline,metampicillinsalt,metampicillinum,micinovo,ocelina,pangocilin,probiotic,relyothenate,ruticina,rutizina,sedomycin,serfabiotic,suvipen,viderpen,viderpin,vioplex</t>
         </is>
       </c>
       <c r="J265">
@@ -16766,7 +16766,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>acetohmt,aminoform,aminoformaldehyde,ammoform,ammonioformaldehyde,antihydral,cystamin,cystex,cystogen,duirexol,ekagomh,esametilentetramina,formamine,formin,heksak,heraxuts,heterin,hexab,hexaform,hexaloids,hexamethylamine,hexamethylenamine,hexamethyleneamine,hexamethylentetramin,hexamine,hexaminesilver,hexaminesuperfine,hexaminum,hexasan,hexilmethylenamine,hmt,mandelamine,metenamina,metenamine,methamin,methenamin,methenaminesilver,methenaminum,metramine,naphthamine,noccelerh,preparationaf,resotropin,sancelerh,sancelerht,silvermethenamine,uramin,uratrine,urisol,uritone,urodeine,urotropin,urotropine,vesaloin,vesalvine,xametrin</t>
+          <t>aminoform,aminoformaldehyde,ammoform,ammonioformaldehyde,antihydral,carin,cystamin,cystex,cystogen,duirexol,esametilentetramina,formamine,formin,grasselerator,heterin,hexaform,hexaloids,hexamethylamine,hexamethylenamine,hexamethyleneamine,hexamethylentetramin,hexamine,hexaminum,hexasan,hexilmethylenamine,metenamina,metenamine,methamin,methamine,methenamin,methenaminum,metramine,naphthamine,pellurin,resotropin,uramin,urasal,uratrine,urisol,uritone,urodeine,urotropin,urotropine,vesaloin,xametrin</t>
         </is>
       </c>
       <c r="J266">
@@ -16830,7 +16830,7 @@
       </c>
       <c r="I267" t="inlineStr">
         <is>
-          <t>dimocillin,metacillin,methcilline,methicillin,methicillinum,methycillin,meticilina,meticillina,meticilline,meticillinum,staphcillin</t>
+          <t>belfacillin,celbenin,celpilline,cinopenil,dimocillin,estafcilina,flabelline,lucopenin,metacillin,methcillin,methicillin,methicillinanhydrous,methicillinhydrate,methicillinsalt,methicillinum,methycillin,meticilina,meticillina,meticilline,meticillinsalt,meticillinum,penaureus,penysol,staficyn,staphcillin,synticillin</t>
         </is>
       </c>
       <c r="J267" t="e">
@@ -17010,7 +17010,7 @@
       </c>
       <c r="I270" t="inlineStr">
         <is>
-          <t>acromona,anagiardil,arilin,atrivyl,danizol,deflamon,donnan,efloran,elyzol,entizol,flagemona,flagesol,flagil,flagyl,flagyler,flagyliv,flagylivrtu,flazol,flegyl,florazole,fossyol,giatricol,gineflavir,helidac,mepagyl,meronidal,methronidazole,metric,metrocream,metrodzhil,metrogel,metrogyl,metroiv,metrolag,metrolotion,metrolyl,metromidol,metronidaz,metronidazol,metronidazoleusp,metronidazolo,metronidazolum,metrotop,metrozine,metryl,mexibol,mexibolsilanes,monagyl,monasin,nidagel,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosased,sanatrichom,satric,takimetol,trichazol,trichex,trichobrol,trichocide,trichocordes,trichomol,trichopal,trichopol,tricocet,tricom,tricowasb,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
+          <t>acromona,anagiardil,arilin,atrivyl,bexon,clont,danizol,deflamon,donnan,efloran,elyzol,entizol,eumin,flagemona,flagesol,flagil,flagyl,flazol,flegyl,florazole,fossyol,giatricol,gineflavir,givagil,hydroxydimetridazole,hydroxymetronidazole,izoklion,klion,klont,mepagyl,meronidal,methronidazole,metric,metrolag,metrolyl,metromidol,metronidaz,metronidazol,metronidazolo,metronidazolum,metroplex,metrotop,mexibol,monagyl,monasin,nalox,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosaced,rosased,sanatrichom,satric,takimetol,trichazol,trichex,trichobrol,trichocide,trichomol,trichopal,trichopol,tricocet,tricom,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
         </is>
       </c>
       <c r="J270">
@@ -17076,7 +17076,7 @@
       </c>
       <c r="I271" t="inlineStr">
         <is>
-          <t>mezlin,mezlocilina,mezlocillinacid,mezlocilline,mezlocillinsodium,mezlocillinum,multocillin</t>
+          <t>baycipen,baypen,mezlin,mezlocilina,mezlocilline,mezlocillinsalt,mezlocillinum,multocillin</t>
         </is>
       </c>
       <c r="J271" t="e">
@@ -17198,7 +17198,7 @@
       </c>
       <c r="I273" t="inlineStr">
         <is>
-          <t>mycamine</t>
+          <t>fungard,funguard,micafungina,micafunginsalt,mycamine</t>
         </is>
       </c>
       <c r="J273" t="e">
@@ -17262,7 +17262,7 @@
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>aflorix,albistat,andergin,brentan,conofite,dactarin,daktarin,daktariniv,florid,lotriminaf,micantin,miconasilnitrate,miconazol,miconazolebase,miconazolo,miconazolum,micozole,minostate,monista,monistat,monistativ,oravig,vusion,zimybase,zimycan</t>
+          <t>aflorix,albistat,andergin,brentan,conofite,dactarin,florid,micantin,miconazol,miconazolo,miconazolum,micozole,minostate,monazole,monista,monistat,oravig,vusion,zimybase,zimycan</t>
         </is>
       </c>
       <c r="J274">
@@ -17324,7 +17324,7 @@
       </c>
       <c r="I275" t="inlineStr">
         <is>
-          <t>gentamicinc,micromicin,micromycin,micronomicina,micronomicine,micronomicinum,sagamicin,santemycin</t>
+          <t>micromicin,micromycin,micronomicina,micronomicine,micronomicinum,sagamicin,santemycin</t>
         </is>
       </c>
       <c r="J275" t="e">
@@ -17386,7 +17386,7 @@
       </c>
       <c r="I276" t="inlineStr">
         <is>
-          <t>aboren,espinomycina,macropen,madecacine,medemycin,midecamicina,midecamycina,midecamycine,midecamycinum,midecin,momicine,mydecamycin,myoxam,normicina,rubimycin,turimycinp</t>
+          <t>macropen,madecacine,medemycin,midecamicina,midecamycine,midecamycinum,midecin,momicine,mydecamycin,myoxam,normicina,rubimycin</t>
         </is>
       </c>
       <c r="J276">
@@ -17510,7 +17510,7 @@
       </c>
       <c r="I278" t="inlineStr">
         <is>
-          <t>akamin,aknemin,borymycin,dynacin,klinomycin,minociclina,minocin,minocline,minocyclin,minocyclinum,minocyn,minoderm,minomycin,sebomin,solodyn,vectrin</t>
+          <t>acnez,arestin,borymycin,dynacin,lederderm,minociclina,minocin,minocline,minocyclin,minocyclinum,minocyn,minomax,minomycin,minoz,mynocine,periocline,solodyn,vectrin,ximino</t>
         </is>
       </c>
       <c r="J278">
@@ -17576,7 +17576,7 @@
       </c>
       <c r="I279" t="inlineStr">
         <is>
-          <t>acecamycin,macroral,midecamycinacetate,miocamen,miocamycine,miokamycin,myocamicin,ponsinomycin</t>
+          <t>acecamycin,macroral,miocamen,miocamycine,miokamycin,mosil,myocamicin,ponsinomycin</t>
         </is>
       </c>
       <c r="J279">
@@ -17636,7 +17636,7 @@
       </c>
       <c r="I280" t="inlineStr">
         <is>
-          <t>monensinsodium,sodiummonensin</t>
+          <t>coban,elancoban,monelan,monensin,monensina,monensine,monensinum,monovet,romensin,rumensin</t>
         </is>
       </c>
       <c r="J280" t="e">
@@ -17698,7 +17698,7 @@
       </c>
       <c r="I281" t="inlineStr">
         <is>
-          <t>morfazinamide,morfazinammide,morfgazinamide,morinamida,morinamidehcl,morinamidum,morphazinamid,morphazinamide,piazofolina,piazolin,piazolina</t>
+          <t>morfazinamide,morfazinammide,morfgazinamide,morinamida,morinamidum,morphazinamid,morphazinamide,piazofolina,piazolin,piazolina</t>
         </is>
       </c>
       <c r="J281" t="e">
@@ -17760,7 +17760,7 @@
       </c>
       <c r="I282" t="inlineStr">
         <is>
-          <t>actira,avelox,aveloxiv,avolex,izilox,moxeza,moxifloxacine,moxivig,vigamox,zimoxin</t>
+          <t>actira,actura,avalox,avelox,avolex,izilox,moxeza,moxifloxacine,moxifloxacino,octegra,vegamox,vigamox,zimoxin</t>
         </is>
       </c>
       <c r="J282">
@@ -17822,7 +17822,7 @@
       </c>
       <c r="I283" t="inlineStr">
         <is>
-          <t>bactoderm,bactroban,bactrobannasal,bactrobanointment,centany,mupirocina,mupirocine,mupirocinum,plasimine,pseudomonicacid,pseudomonicacida,turixin</t>
+          <t>bactoderm,bactroban,centany,mupirocina,mupirocine,mupirocinum,plasimine,turixin</t>
         </is>
       </c>
       <c r="J283" t="e">
@@ -17996,7 +17996,7 @@
       </c>
       <c r="I286" t="inlineStr">
         <is>
-          <t>nafcilina,nafcilline,nafcillinsodium,nafcillinum,nallpen,naphcillin,unipen</t>
+          <t>nafcil,nafcilin,nafcilina,nafcillinanhydrous,nafcilline,nafcillinhydrate,nafcillinmonohydrate,nafcillinsalt,nafcillinum,naftopen,nallpen,naphcillin,naphthicillin,unipen</t>
         </is>
       </c>
       <c r="J286" t="e">
@@ -18118,7 +18118,7 @@
       </c>
       <c r="I288" t="inlineStr">
         <is>
-          <t>acidenalidixico,acidenalidixique,acidonalidissico,acidonalidixico,acidumnalidixicum,betaxina,dixiben,dixinal,eucisten,eucistin,innoxalomn,innoxalon,jicsron,kusnarin,naldixicacid,nalidicacid,nalidicron,nalidixan,nalidixane,nalidixate,nalidixatesodium,nalidixic,nalidixicacid,nalidixin,nalidixinicacid,nalidixinsaure,nalitucsan,nalurin,narigix,naxuril,neggram,negram,nevigramon,nicelate,nogram,poleon,sicmylon,specifen,specifin,unaserus,uralgin,uriben,uriclar,urisal,urodixin,uroman,uroneg,uronidix,uropan,wintomylon,wintron</t>
+          <t>amfonelinsaeure,baktogram,betaxina,chemiurin,cybis,dixiben,dixilina,dixinal,eucisten,eucistin,innoxalomn,innoxalon,jicsron,kusnarin,nalidicron,nalidixan,nalidixane,nalidixate,nalidixateanhydrous,nalidixic,nalidixin,nalidixinsaure,nalitucsan,nalix,nalurin,narigix,naxuril,negram,nevigramon,nicelate,nogram,poleon,sicmylon,specifen,specifin,unaserus,uralgin,uriben,uriclar,urisal,urodixin,uroman,uroneg,uronidix,uropan,wintomylon,wintron</t>
         </is>
       </c>
       <c r="J288">
@@ -18236,7 +18236,7 @@
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>monteban,narasina,narasine,narasino,narasinum,narasul</t>
+          <t>monteban,narasine,narasino,narasinum,skycis</t>
         </is>
       </c>
       <c r="J290" t="e">
@@ -18360,7 +18360,7 @@
       </c>
       <c r="I292" t="inlineStr">
         <is>
-          <t>actilin,actiline,antibiotique,bycomycin,dekamyciniii,endomixin,enterfram,fradiomycin,fradiomycinb,fradiomycinum,framicetina,framidal,framycetine,framycetinsulfate,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycinb,neomycinbsulfate,neomycine,neomycinsolution,neomycinsulfate,neomycinsulphate,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycinpowderv</t>
+          <t/>
         </is>
       </c>
       <c r="J292">
@@ -18426,7 +18426,7 @@
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>netillin,netilmicina,netilmicine,netilmicinsulfate,netilmicinum,netilyn,netira,nettacin,vectacin</t>
+          <t>netillin,netilmicina,netilmicine,netilmicinum,netilyn,netira,netromicine,netromycin,nettacin,ntromicine,ntromycin,vectacin,zetamicin</t>
         </is>
       </c>
       <c r="J293">
@@ -18488,7 +18488,7 @@
       </c>
       <c r="I294" t="inlineStr">
         <is>
-          <t>nicarb,nicarbasin,nicarbazine,nicoxin,nicrazin,nicrazine,nirazin</t>
+          <t>nicarb,nicarbasin,nicarbazine,nicarmix,nicoxin,nicrazin,nicrazine,nirazin</t>
         </is>
       </c>
       <c r="J294" t="e">
@@ -18608,7 +18608,7 @@
       </c>
       <c r="I296" t="inlineStr">
         <is>
-          <t>levantin,nifurtoinolo,nifurtoinolum,urfadin,urfadine,urfadyn</t>
+          <t>levantin,nifurmazol,nifurmazole,nifurmazolo,nifurmazolum,nifurtoinolo,nifurtoinolum,urfadin,urfadine,urfadyn</t>
         </is>
       </c>
       <c r="J296">
@@ -18668,7 +18668,7 @@
       </c>
       <c r="I297" t="inlineStr">
         <is>
-          <t>adrovet,alinia,aztnitazoxanide,colufase,cryptaz,dexidex,heliton,kidonax,nitaxozanid,nitaxozanide,nitazox,nitazoxamide,nitazoxanid,nitazoxanida,nitazoxanidum,nitrazoxanide,omniparax,pacovanton,paramix,taenitaz</t>
+          <t>alinia,benzamide,colufase,cryptaz,daxon,dexidex,heliton,kidonax,nitax,nitaxozanid,nitaxozanide,nitazox,nitazoxamide,nitazoxanid,nitazoxanida,nitazoxanidum,nitrazoxanide,pacovanton,paramix,phavic</t>
         </is>
       </c>
       <c r="J297">
@@ -18732,7 +18732,7 @@
       </c>
       <c r="I298" t="inlineStr">
         <is>
-          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fuamed,furabid,furachel,furadantin,furadantinamc,furadantine,furadantinemc,furadantinretard,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furadoxyl,furalan,furaloid,furantoin,furantoina,furatoin,furedan,furina,furobactina,furodantin,furophent,gerofuran,ioussaixoo,ituran,ivadantin,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifurantin,nifuretten,nitoin,nitrex,nitrofuradantin,nitrofurantion,nitrofurantoina,nitrofurantoine,nitrofurantoinmacro,nitrofurantoinum,novofuran,orafuran,parfuran,phenurin,piyeloseptyl,siraliden,trantoin,uerineks,urantoin,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
+          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fuamed,furabid,furachel,furadantin,furadantine,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furalan,furaloid,furantoin,furantoina,furatoin,furedan,furina,furobactina,furodantin,gerofuran,ituran,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifuraden,nifuradene,nifuradeno,nifuradenum,nifuradine,nifurantin,nifuretten,nitoin,nitrex,nitrofuradantin,nitrofurantoina,nitrofurantoine,nitrofurantoinum,novofuran,orafuran,oxafuradene,oxafurandene,oxifuradene,oxyfuradene,parfuran,phenurin,renafur,siraliden,trantoin,uerineks,urantoin,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
         </is>
       </c>
       <c r="J298">
@@ -18792,7 +18792,7 @@
       </c>
       <c r="I299" t="inlineStr">
         <is>
-          <t>acutol,aldomycin,alfucin,amifur,babrocid,becafurazone,biofuracina,biofurea,chemofuran,chixin,cocafurin,coxistat,dermofural,dymazone,dynazone,eldezol,fedacin,flavazone,fracine,furacilin,furacilinum,furacillin,furacin,furacine,furacinetten,furacoccid,furacort,furacycline,furaderm,furagent,furalcyn,furaldon,furalone,furametral,furaplast,furaseptyl,furaskin,furatsilin,furaziline,furazin,furazina,furazolw,furazone,furazyme,furesol,furfurin,furosem,fuvacillin,hemofuran,ibiofural,mammex,mastofuran,monafuracin,monafuracis,monofuracin,nfzmix,nifucin,nifurid,nifuzon,nitrofural,nitrofuralum,nitrofuran,nitrofurane,nitrofurazan,nitrofurazonum,nitrofurol,nitrozone,otofural,otofuran,rivafurazon,sanfuran,vabrocid,vadrocid,yatrocin</t>
+          <t>acutol,aldomycin,alfucin,amifur,babrocid,becafurazone,biofuracina,biofurea,chemofuran,chixin,cocafurin,coxistat,dermofural,dymazone,dynazone,eldezol,fedacin,flavazone,fracine,furacilin,furacilinum,furacillin,furacin,furacine,furacinetten,furacoccid,furacort,furacycline,furaderm,furagent,furalcyn,furaldon,furalone,furametral,furaplast,furaseptyl,furaskin,furatsilin,furaziline,furazin,furazina,furazone,furazyme,furesol,furosem,fuvacillin,hemofuran,hydrazinecarboxamide,ibiofural,mammex,mastofuran,monafuracin,monafuracis,monofuracin,nefco,nifucin,nifurid,nifuzon,nitrofural,nitrofuralum,nitrofuran,nitrofurane,nitrofurazan,nitrofurazonum,nitrofurol,nitrozone,otofural,otofuran,rivafurazon,rivopon,sanfuran,semioxamazide,vabrocid,vadrocid,yatrocin</t>
         </is>
       </c>
       <c r="J299" t="e">
@@ -18854,7 +18854,7 @@
       </c>
       <c r="I300" t="inlineStr">
         <is>
-          <t>galinok,isinok,nibiol,niceneforte,nitroxlina,nitroxolin,nitroxolina,nitroxolinum,notroxoline,noxibiol</t>
+          <t>galinok,isinok,nibiol,nicene,nitroxlina,nitroxolin,nitroxolina,nitroxolinum,noxibiol,noxin</t>
         </is>
       </c>
       <c r="J300">
@@ -18918,7 +18918,7 @@
       </c>
       <c r="I301" t="inlineStr">
         <is>
-          <t>baccidal,barazan,chibroxin,chibroxine,chibroxol,fulgram,gonorcin,lexinor,nolicin,noracin,noraxin,norflo,norfloxacine,norfloxacino,norfloxacinum,norocin,noroxin,noroxine,norxacin,sebercim,uroxacin,utinor,zoroxin</t>
+          <t>baccidal,barazan,chibroxin,chibroxine,chibroxol,fulgram,gonorcin,lexinor,noflo,nolicin,noracin,noraxin,norflo,norfloxacine,norfloxacino,norfloxacinum,norocin,noroxin,noroxine,norxacin,sebercim,uroxacin,utinor,zoroxin</t>
         </is>
       </c>
       <c r="J301">
@@ -19218,7 +19218,7 @@
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>albamix,albamycin,cardelmycin,cathocin,cathomycin,crystallinicacid,inamycin,novobiocina,novobiocine,novobiocinum,robiocina,sirbiocina,spheromycin,stilbiocina,streptonivicin</t>
+          <t>albadry,albamix,albamycin,biotexin,cardelmycin,cardelmycinsalt,cathocin,cathomycin,inabiocin,inamycin,novobiocina,novobiocine,novobiocinsalt,novobiocinum,robiocina,sirbiocina,spheromycin,stilbiocina,streptonivicin,streptonivicinsalt,vulcamicina,vulcamycin,vulkamycin</t>
         </is>
       </c>
       <c r="J306" t="e">
@@ -19276,7 +19276,7 @@
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>biofanal,candexlotion,comycin,diastatin,herniocid,moronal,myconystatin,mycostatin,mycostatinpastilles,mykinac,mykostatyna,nilstat,nistatin,nistatina,nyamyc,nyotran,nyotrantrademark,nystaform,nystan,nystatina,nystatine,nystating,nystatinhydrate,nystatinlf,nystatinum,nystatyna,nystavescent,nystex,nystop,stamycin,terrastatin,zydine</t>
+          <t>biofanal,diastatin,herniocid,moronal,myconystatin,mycostatin,mykostatyna,nilstat,nistatin,nistatina,nyotran,nystan,nystatyna,nystavescent,nystex,stamycin</t>
         </is>
       </c>
       <c r="J307">
@@ -19340,7 +19340,7 @@
       </c>
       <c r="I308" t="inlineStr">
         <is>
-          <t>bactocin,danoflox,dextrofloxacin,effexin,exocin,exocine,flobacin,flodemex,flotavid,flovid,floxal,floxil,floxin,floxinotic,floxstat,fugacin,inoflox,kinflocin,kinoxacin,levofloxacinhcl,liflox,loxinter,marfloxacin,medofloxine,mergexin,monoflocet,novecin,nufafloqo,occidal,ocuflox,oflocee,oflocet,oflocin,oflodal,oflodex,oflodura,ofloxacina,ofloxacine,ofloxacino,ofloxacinotic,ofloxacinum,ofloxin,onexacin,operan,orocin,otonil,oxaldin,pharflox,praxin,puiritol,qinolon,quinolon,quotavil,sinflo,tabrin,taravid,tariflox,tarivid,telbit,tructum,urotarivid,viotisone,visiren,zanocin</t>
+          <t>exocin,exocine,flobacin,floxil,floxin,monoflocet,ocuflox,oflocet,ofloxacina,ofloxacine,ofloxacino,ofloxacinum,ofloxaxin,oxaldin,tarivid,visiren,zanocin</t>
         </is>
       </c>
       <c r="J308">
@@ -19468,7 +19468,7 @@
       </c>
       <c r="I310" t="inlineStr">
         <is>
-          <t>amimycin,landomycin,matromycin,oleandomicina,oleandomycina,oleandomycine,oleandomycinum,romicil</t>
+          <t>amimycin,landomycin,matromycin,oleandomicina,oleandomycine,oleandomycinum,romicil</t>
         </is>
       </c>
       <c r="J310">
@@ -19590,7 +19590,7 @@
       </c>
       <c r="I312" t="inlineStr">
         <is>
-          <t>numoquin,optoquine</t>
+          <t>aflukin,auriquin,biquinate,chinidin,chinidine,chinimetten,chinin,chinine,conchinin,conchinine,conquinine,dentojel,dihydrochinidin,dihydroquinidine,dihydroquinine,hydroconchinine,hydroconquinine,hydroquinidine,kinidin,numoquin,optochine,optoquine,pitayine,qualaquin,quinaglute,quine,quinicardine,quinidex,quinidine,quiniduran,quinindine,quinine,quinineanhydrous,quinora,quinsan,rezquin</t>
         </is>
       </c>
       <c r="J312" t="e">
@@ -19648,7 +19648,7 @@
       </c>
       <c r="I313" t="inlineStr">
         <is>
-          <t/>
+          <t>orbax</t>
         </is>
       </c>
       <c r="J313" t="e">
@@ -19710,7 +19710,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>kimyrsa</t>
+          <t/>
         </is>
       </c>
       <c r="J314" t="e">
@@ -19830,7 +19830,7 @@
       </c>
       <c r="I316" t="inlineStr">
         <is>
-          <t>madelen,ornidal,ornidazol,ornidazolum,tiberal</t>
+          <t>levornidazole,madelen,ornidal,ornidazol,ornidazolum,tiberal</t>
         </is>
       </c>
       <c r="J316">
@@ -19896,7 +19896,7 @@
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t/>
+          <t>quilseconazole,vivijoa</t>
         </is>
       </c>
       <c r="J317">
@@ -19960,7 +19960,7 @@
       </c>
       <c r="I318" t="inlineStr">
         <is>
-          <t>bactocill,ossacillina,oxacilina,oxacilline,oxacillinsodium,oxacillinum,oxazocillin,oxazocilline,prostaphlin,prostaphlyn,sodiumoxacillin</t>
+          <t>bactocill,bristopen,cryptocillin,micropenin,ossacillina,oxabel,oxabelsalt,oxacilina,oxacillinanhydrous,oxacilline,oxacillinhydrate,oxacillinsalt,oxacillinum,oxazocillin,oxazocilline,penstapho,prostaphlin,prostaphlyn,resistopen,stapenor</t>
         </is>
       </c>
       <c r="J318">
@@ -20084,7 +20084,7 @@
       </c>
       <c r="I320" t="inlineStr">
         <is>
-          <t>acideoxolinique,acidoossolico,acidooxolinico,acidumoxolinicum,aqualinic,cistopax,dioxacin,emyrenil,gramurin,inoxyl,nidantin,oksaren,orthurine,ossian,oxoboi,oxolinic,oxolinicacid,pietil,prodoxal,prodoxol,starner,tiurasin,ultibid,urinox,uritrate,urotrate,uroxol,utibid</t>
+          <t>aqualinic,cistopax,dioxacin,emyrenil,gramurin,inoxyl,nidantin,oksaren,orthurine,ossian,oxoboi,oxolinic,pietil,prodoxal,prodoxol,starner,tiurasin,ultibid,urinox,uritrate,urotrate,uroxol,utibid</t>
         </is>
       </c>
       <c r="J320">
@@ -20148,7 +20148,7 @@
       </c>
       <c r="I321" t="inlineStr">
         <is>
-          <t>adamycin,berkmycen,biostat,biostatpa,bisolvomycin,dabicycline,dalimycin,embryostat,fanterrin,galsenomycin,geomycin,geotilin,hydroxytetracyclinum,imperacin,lenocycline,macocyn,medamycin,mepatar,oksisyklin,ossitetraciclina,oxacycline,oxitetraciclina,oxitetracyclin,oxitetracycline,oxitetracyclinum,oxydon,oxymycin,oxymykoin,oxypam,oxysteclin,oxyterracin,oxyterracine,oxyterracyne,oxytetracid,oxytetracyclin,oxytetracyclinebase,oxytetracyclinum,proteroxyna,riomitsin,ryomycin,solkaciclina,stecsolin,stevacin,tarocyn,tarosin,teravit,terrafungine,terramitsin,terramycin,terramycine,terramycinim,tetran,unimycin,ursocyclin,ursocycline,vendarcin</t>
+          <t>achromycin,actisite,adamycin,artomycin,berkmycen,biostat,bristacycline,cancycline,cyclopar,dabicycline,diacycine,dumocyclin,embryostat,fanterrin,galsenomycin,geomycin,geotilin,hostacycline,hydroxytetracyclinum,lenocycline,macocyn,medamycin,mephacyclin,nitox,oksisyklin,ossitetraciclina,oxitetraciclina,oxitetracyclin,oxitetracycline,oxitetracyclinum,oxymycin,oxypam,oxyterracin,oxyterracine,oxyterracyne,oxytetracid,oxytetracyclin,oxytetracyclinum,paltet,partrex,pennox,piracaps,proteroxyna,qidtet,quadracycline,quatrex,remicyclin,retet,ricycline,riomitsin,ryomycin,solkaciclina,stevacin,stilciclina,subamycin,sumycin,supramycin,sustamycin,tarocyn,tarosin,tefilin,teline,telotrex,teravit,terrafungine,terramitsin,terramycine,tetrabakat,tetrabid,tetrablet,tetracaps,tetracompren,tetrakap,tetralution,tetramavan,tetramed,tetran,tetrosol,topicycline,triphacyclin,unicin,ursocyclin,ursocycline,vetquamycin</t>
         </is>
       </c>
       <c r="J321">
@@ -20208,7 +20208,7 @@
       </c>
       <c r="I322" t="inlineStr">
         <is>
-          <t>ozadub,ozenoxacincream</t>
+          <t/>
         </is>
       </c>
       <c r="J322" t="e">
@@ -20266,7 +20266,7 @@
       </c>
       <c r="I323" t="inlineStr">
         <is>
-          <t>aminopar,aminosalicylic,aminosalicylicacid,aminosalyl,aminox,apacil,deapasil,entepas,ferrosan,gabbropas,granupas,helipidyl,hellipidyl,neopasalate,osacyl,pamacyl,pamisyl,paramycin,parasal,parasalicil,parasalindon,pasalon,pasara,pascorbic,pasdium,pasergranules,paskalium,pasmed,pasnodia,pasolac,propasa,rezipas,teebacin</t>
+          <t/>
         </is>
       </c>
       <c r="J323" t="e">
@@ -20324,7 +20324,7 @@
       </c>
       <c r="I324" t="inlineStr">
         <is>
-          <t>panipenembetamipron,panipenemum,penipanem</t>
+          <t>carbenin,panipenemum,penipanem</t>
         </is>
       </c>
       <c r="J324" t="e">
@@ -20384,7 +20384,7 @@
       </c>
       <c r="I325" t="inlineStr">
         <is>
-          <t>aminosidin,aminosidine,aminosidinei,aminosidinesulfate,amminosidin,crestomycin,estomycin,gabbromicina,gabbromycin,gabromycin,humatin,humycin,hydroxymycin,hydroxymycinsulfate,monomycin,monomycina,neomycine,paramomycin,paramomycinsulfate,paromomicina,paromomycine,paromomycini,paromomycinum,paucimycin,paucimycinum,quintomycinc</t>
+          <t>aminosidin,amminosidin,crestomycin,estomycin,gabbromycin,gabromycin,humatin,humycin,hydroxymycin,monomycin,paramomycin,paromomicina,paromomycine,paromomycinum,paucimycin,paucimycinum</t>
         </is>
       </c>
       <c r="J325">
@@ -20512,7 +20512,7 @@
       </c>
       <c r="I327" t="inlineStr">
         <is>
-          <t>abactal,labocton,pefloxacine,pefloxacinium,pefloxacino,pefloxacinum,perfloxacin,silverpefloxacin</t>
+          <t>labocton,pefbid,pefloxacine,pefloxacinium,pefloxacino,pefloxacinum,pefocin,pefran,pelox</t>
         </is>
       </c>
       <c r="J327">
@@ -20636,7 +20636,7 @@
       </c>
       <c r="I329" t="inlineStr">
         <is>
-          <t>hydroxymethyl,penamecilina,penamecillina,penamecilline,penamecillinum</t>
+          <t>havapen,hydroxymethyl,penamecilina,penamecillina,penamecilline,penamecillinum</t>
         </is>
       </c>
       <c r="J329">
@@ -20874,7 +20874,7 @@
       </c>
       <c r="I333" t="inlineStr">
         <is>
-          <t>pentisomicina,pentisomicine,pentisomicinum</t>
+          <t>mutamicin,mutamycin,pentisomicina,pentisomicine,pentisomicinum</t>
         </is>
       </c>
       <c r="J333" t="e">
@@ -20990,7 +20990,7 @@
       </c>
       <c r="I335" t="inlineStr">
         <is>
-          <t/>
+          <t>cytolex,mangainin</t>
         </is>
       </c>
       <c r="J335" t="e">
@@ -21052,7 +21052,7 @@
       </c>
       <c r="I336" t="inlineStr">
         <is>
-          <t>feneticilina,feneticillin,feneticillina,feneticilline,kphenethicillin,phenethicilin,phenethicillinum,pheneticilline,pheneticillinum,phenoxypc,potassiumpenicillin,synthepen</t>
+          <t>alfacillin,alticina,antibiocin,arcacil,arcasin,astracillin,bendralan,beromycin,brocsil,broxil,chemipen,cliacil,darcil,feneticilina,feneticillin,feneticillina,feneticilline,fenocin,icipen,isocillin,ispenoral,kavepenin,maxipen,optipen,oralopen,orapen,ospeneff,pedipen,penagen,pencompren,penemve,peniplus,penova,pensig,penvikal,phenethicilin,phenethicillin,phenethicillinum,pheneticilline,pheneticillinum,primcillin,priospen,roscopenin,semopen,suspen,synapen,syncillin,synerpenin,synthecillin,synthecilline,synthepen,triospen,vamosyn,veetids,vepen</t>
         </is>
       </c>
       <c r="J336">
@@ -21116,7 +21116,7 @@
       </c>
       <c r="I337" t="inlineStr">
         <is>
-          <t>acipenv,apocillin,apopen,beromycin,calcipen,compocillinv,crystapenv,distaquainev,eskacillianv,eskacillinv,fenacilin,fenospen,meropenin,oracillin,oratren,pcpenvk,penicillinv,phenocillin,phenomycilline,phenopenicillin,robicillin,rocilin,stabicillin,vebecillin,veetids,vegacillin</t>
+          <t>apopen,calcipen,fenacilin,fenospen,meropenin,oracillin,oracilline,oratren,orocillin,ospen,phenocillin,phenomycilline,phenopenicillin,rocilin,stabicillin,vebecillin</t>
         </is>
       </c>
       <c r="J337">
@@ -21176,7 +21176,7 @@
       </c>
       <c r="I338" t="inlineStr">
         <is>
-          <t>delvocid,delvolan,delvopos,mycophyt,myprozine,natacyn,natafucin,natamicina,natamycin,natamycine,natamycinum,pimafucin,pimaracin,pimaricine,pimarizin,synogil,tennecetin</t>
+          <t>delvocid,delvolan,delvopos,mycophyt,myprozine,natacyn,natafucin,natajen,natamatrix,natamax,natamicina,natamycin,natamycine,natamycinum,pimafucin,pimaracin,pimaricine,pimarizin,synogil,tennecetin</t>
         </is>
       </c>
       <c r="J338" t="e">
@@ -21238,7 +21238,7 @@
       </c>
       <c r="I339" t="inlineStr">
         <is>
-          <t>acidepipemidique,acidopipemidico,acidumpipemidicum,deblaston,dolcol,filtrax,pipedac,pipemid,pipemidate,pipemidic,pipemidicacid,pipram,pipurin,tractur,uromidin,urosten,uroval</t>
+          <t>deblaston,dolcol,filtrax,karunomazin,memento,nuril,palin,pipedac,pipemid,pipemidate,pipemidic,pipemidicacid,pipram,pipurin,pyrido,tractur,uromidin,urosten,uroval</t>
         </is>
       </c>
       <c r="J339">
@@ -21302,7 +21302,7 @@
       </c>
       <c r="I340" t="inlineStr">
         <is>
-          <t>isipen,pentcillin,peperacillin,peracin,piperacilina,piperacillina,piperacilline,piperacillinhydrate,piperacillinna,piperacillinsodium,piperacillinum,pipercillin,pipracil,pipril,tazocin</t>
+          <t>penmalin,pentcillin,peperacillin,peracin,piperacilina,piperacillina,piperacilline,piperacillinhydrate,piperacillinum,pipercillin,pipracil,tazocin</t>
         </is>
       </c>
       <c r="J340" t="e">
@@ -21424,7 +21424,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>tazocel,tazocillin,tazocin,zosyn</t>
+          <t>piptazobactam,tazobac,tazonam,zobactin,zosyn</t>
         </is>
       </c>
       <c r="J342" t="e">
@@ -21604,7 +21604,7 @@
       </c>
       <c r="I345" t="inlineStr">
         <is>
-          <t>acidepiromidique,acidopiromidico,acidumpiromidicum,actrunc,bactramyl,enterol,gastrurol,panacid,pirodal,piromidate,piromidicacid,pyrido,reelon,septural,urisept,uropir,zaomeal</t>
+          <t>bactramyl,enterol,gastrurol,panacid,pirodal,piromidate,reelon,septural,urisept,uropir,zaomeal</t>
         </is>
       </c>
       <c r="J345">
@@ -21668,7 +21668,7 @@
       </c>
       <c r="I346" t="inlineStr">
         <is>
-          <t>berocillin,pivaloylampicillin,pivampicilina,pivampicilline,pivampicillinum,pondocillin</t>
+          <t>pivaloylampicillin,pivampicilina,pivampicilline,pivampicillinum</t>
         </is>
       </c>
       <c r="J346">
@@ -21732,7 +21732,7 @@
       </c>
       <c r="I347" t="inlineStr">
         <is>
-          <t>amdinocillinpivoxil,coactabs,hydroxymethyl,pivmecilinamo,pivmecillinamhcl,pivmecillinamum</t>
+          <t>coactabs,melysin,pivamdinocillin,pivmecilinamo,pivmecillinamum,selexid</t>
         </is>
       </c>
       <c r="J347">
@@ -21854,7 +21854,7 @@
       </c>
       <c r="I349" t="inlineStr">
         <is>
-          <t>polimixinab,polumyxinb,polymixinb,polymyxineb</t>
+          <t>aerosporin</t>
         </is>
       </c>
       <c r="J349">
@@ -21978,7 +21978,7 @@
       </c>
       <c r="I351" t="inlineStr">
         <is>
-          <t>noxafil,posaconazolesp,posconazole</t>
+          <t>noxafil,schering,spriafil</t>
         </is>
       </c>
       <c r="J351">
@@ -22098,7 +22098,7 @@
       </c>
       <c r="I353" t="inlineStr">
         <is>
-          <t>remafloxacin</t>
+          <t>premafloxacine,premafloxacino,remafloxacin</t>
         </is>
       </c>
       <c r="J353" t="e">
@@ -22160,7 +22160,7 @@
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t>oxazine</t>
+          <t/>
         </is>
       </c>
       <c r="J354">
@@ -22220,7 +22220,7 @@
       </c>
       <c r="I355" t="inlineStr">
         <is>
-          <t/>
+          <t>chinopricin,debrycin,primicina,primycine</t>
         </is>
       </c>
       <c r="J355" t="e">
@@ -22282,7 +22282,7 @@
       </c>
       <c r="I356" t="inlineStr">
         <is>
-          <t>eskalinv,mikamycin,mikamycine,mikamycinum,ostreogrycinum,pristinamycine,pristinamycinum,stafac,stafytracine,staphylomycin,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamycin,virginiamycina,virginiamycinum</t>
+          <t>eskalin,micamicina,mikamycin,mikamycine,mikamycinum,ostreogricina,ostreogrycin,ostreogrycine,ostreogrycinum,pristinamicina,pristinamycine,pristinamycinum,pyostacine,stafac,stafytracine,stajac,staphylomycin,stapyocine,starfac,virgimycin,virgimycine,virginiamicina,virginiamycin,virginiamycina,virginiamycinum</t>
         </is>
       </c>
       <c r="J356">
@@ -22346,7 +22346,7 @@
       </c>
       <c r="I357" t="inlineStr">
         <is>
-          <t>depocillin,duphapen,hostacillin,hydracillin,jenacillino,nopcaine,penicillinprocaine,retardillin,vetspen,vitablend</t>
+          <t>afsillin,aquacilina,aquacillin,aquasuspen,avloprocil,cilicaine,crysticillin,depocillin,despacilina,distaquaine,duphapen,duracillin,hostacillin,hydracillin,kabipenin,ledercillin,millicillin,mylipen,neoproc,nopcaine,parencillin,premocillin,procanodia,prostabillin,retardillin,sharcillin,vetspen,vitablend,wycillin</t>
         </is>
       </c>
       <c r="J357" t="e">
@@ -22410,7 +22410,7 @@
       </c>
       <c r="I358" t="inlineStr">
         <is>
-          <t>propicilina,propicilline,propicillinum</t>
+          <t>baycillin,propicilina,propicilline,propicillinum</t>
         </is>
       </c>
       <c r="J358">
@@ -22596,7 +22596,7 @@
       </c>
       <c r="I361" t="inlineStr">
         <is>
-          <t>pruvel,pufloxacindioxolil,quisnon</t>
+          <t>pruvel,quisnon,sword</t>
         </is>
       </c>
       <c r="J361">
@@ -22660,7 +22660,7 @@
       </c>
       <c r="I362" t="inlineStr">
         <is>
-          <t>aldinamid,aldinamide,braccopiral,corsazinmid,dipimide,eprazin,farmizina,isopas,lynamide,novamid,pezetamid,pharozinamide,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,prazina,pyrafat,pyramide,pyrazide,pyrazinamdie,pyrazinamid,pyrazinamidum,pyrazineamide,pyrazinecarboxamide,pyrizinamide,rifafour,rozide,tebrazid,tebrazio,tisamid,unipyranamide,zinamide,zinastat</t>
+          <t>aldinamid,aldinamide,eprazin,farmizina,isopas,novamid,pezetamid,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,pirazinecarboxamide,pyrafat,pyrazide,pyrazinamdie,pyrazinamid,pyrazinamidum,pyrazineamide,pyrizinamide,rifafour,rozide,tebrazid,tisamid,unipyranamide,zinamide</t>
         </is>
       </c>
       <c r="J362">
@@ -22724,7 +22724,7 @@
       </c>
       <c r="I363" t="inlineStr">
         <is>
-          <t/>
+          <t>synercid</t>
         </is>
       </c>
       <c r="J363" t="e">
@@ -22782,7 +22782,7 @@
       </c>
       <c r="I364" t="inlineStr">
         <is>
-          <t>optaflexx,paylean,ractopamina,ractopaminum</t>
+          <t>bufenina,bufenine,buphenin,buphenine,bupheninum,luteonin,nilidrine,nylidrinum,optaflexx,paylean,prepar,ractopamina,ractopaminum,ritodrina,ritodrine,ritodrinium,tomax,utopar,yutopar</t>
         </is>
       </c>
       <c r="J364" t="e">
@@ -22960,7 +22960,7 @@
       </c>
       <c r="I367" t="inlineStr">
         <is>
-          <t>altabax,altargo</t>
+          <t>altabax,altargo,rebapamulin,retapamulina</t>
         </is>
       </c>
       <c r="J367" t="e">
@@ -23018,7 +23018,7 @@
       </c>
       <c r="I368" t="inlineStr">
         <is>
-          <t>biafungin,rezafungincation,rezafunginion</t>
+          <t/>
         </is>
       </c>
       <c r="J368" t="e">
@@ -23144,7 +23144,7 @@
       </c>
       <c r="I370" t="inlineStr">
         <is>
-          <t>dekamyciniv,hetangmycin,ribastamin,ribostamicina,ribostamycine,ribostamycinum,vistamycin,xylostatin</t>
+          <t>exaluren,hetangmycin,ribastamin,ribostamicina,ribostamycine,ribostamycinum,vistamycin,xylostatin</t>
         </is>
       </c>
       <c r="J370" t="e">
@@ -23204,7 +23204,7 @@
       </c>
       <c r="I371" t="inlineStr">
         <is>
-          <t/>
+          <t>ridinilazol</t>
         </is>
       </c>
       <c r="J371" t="e">
@@ -23266,7 +23266,7 @@
       </c>
       <c r="I372" t="inlineStr">
         <is>
-          <t>alfacid,ansamicin,ansamycin,ansatipin,ansatipine,assatipin,mycobutin,rifabutina,rifabutine,rifabutinum</t>
+          <t>alfacid,ansamicin,ansamycins,ansatipin,ansatipine,assatipin,mycobutin,rifabutinum</t>
         </is>
       </c>
       <c r="J372">
@@ -23330,7 +23330,7 @@
       </c>
       <c r="I373" t="inlineStr">
         <is>
-          <t>abrifam,archidyn,arficin,arzide,aztrifampin,benemicin,benemycin,dipicin,doloresum,eremfat,famcin,fenampicin,rifadin,rifadine,rifadiniv,rifagen,rifaldazin,rifaldazine,rifaldin,rifamate,rifamicinamp,rifamor,rifampicina,rifampicine,rifampicinsv,rifampicinum,rifampin,rifamsolin,rifamycinamp,rifapiam,rifaprodin,rifcin,rifinah,rifobac,rifoldin,rifoldine,riforal,rimactan,rimactane,rimactazid,rimactizid,rimazid,rimycin,sinerdol,tubocin</t>
+          <t>abrifam,archidyn,arficin,arzide,benemicin,doloresum,eremfat,famcin,fenampicin,rifadin,rifadine,rifagen,rifaldazin,rifaldazine,rifaldin,rifam,rifamor,rifampicina,rifampicine,rifampicinum,rifampin,rifamsolin,rifapiam,rifaprodin,rifcin,rifinah,rifobac,rifoldin,rifoldine,riforal,rimactan,rimactane,rimactazid,rimactizid,rimazid,sinerdol,tubocin</t>
         </is>
       </c>
       <c r="J373">
@@ -23396,7 +23396,7 @@
       </c>
       <c r="I374" t="inlineStr">
         <is>
-          <t/>
+          <t>isonarif,rifamate,rifamazid</t>
         </is>
       </c>
       <c r="J374" t="e">
@@ -23458,7 +23458,7 @@
       </c>
       <c r="I375" t="inlineStr">
         <is>
-          <t>rifinah,rimactazid</t>
+          <t/>
         </is>
       </c>
       <c r="J375" t="e">
@@ -23644,7 +23644,7 @@
       </c>
       <c r="I378" t="inlineStr">
         <is>
-          <t>aemcolo,rifacin,rifamicina,rifamicinesv,rifamycine,rifamycinum,rifocin,rifocyn,rifomycin,rifomycinsv,tuborin</t>
+          <t>aemcolo,nacimycin,nancimycin,otofa,rifamastene,rifamicina,rifamycine,rifamycinum,rifocin,rifocyn,tuborin</t>
         </is>
       </c>
       <c r="J378">
@@ -23710,7 +23710,7 @@
       </c>
       <c r="I379" t="inlineStr">
         <is>
-          <t>cyclopentylrifampin,prifitin,priftin,rifapentin,rifapentina,rifapentinum</t>
+          <t>prifitin,priftin,rifapentin,rifapentina,rifapentinum</t>
         </is>
       </c>
       <c r="J379">
@@ -23774,7 +23774,7 @@
       </c>
       <c r="I380" t="inlineStr">
         <is>
-          <t>fatroximin,flonorm,lormyx,lumenax,normix,redactiv,rifacol,rifamixin,rifaxidin,rifaximina,rifaximine,rifaximinum,rifaxin,ritacol,spiraxin,xifaxan,xifaxsan</t>
+          <t>fatroximin,flonorm,lormyx,lumenax,normix,rifacol,rifamixin,rifaxidin,rifaximina,rifaximine,rifaximinum,rifaxin,ritacol,spiraxin,xifaxan,xifaxsan</t>
         </is>
       </c>
       <c r="J380">
@@ -23834,7 +23834,7 @@
       </c>
       <c r="I381" t="inlineStr">
         <is>
-          <t/>
+          <t>ritipenemsalt</t>
         </is>
       </c>
       <c r="J381" t="e">
@@ -23892,7 +23892,7 @@
       </c>
       <c r="I382" t="inlineStr">
         <is>
-          <t>ritipenemacoxil</t>
+          <t>penemac</t>
         </is>
       </c>
       <c r="J382" t="e">
@@ -24018,7 +24018,7 @@
       </c>
       <c r="I384" t="inlineStr">
         <is>
-          <t>bristacin,kinteto,reverin,rolitetraciclina,rolitetracyclinum,solvocillin,superciclin,synotodecin,synterin,syntetrex,syntetrin,transcycline,velacicline,velacycline</t>
+          <t>bristacin,colbiocin,kinteto,reverin,revrin,rolitetraciclina,rolitetracyclinum,solvocillin,superciclin,synotodecin,synterin,syntetrex,syntetrin,tetraverin,transcycline,velacicline,velacycline</t>
         </is>
       </c>
       <c r="J384" t="e">
@@ -24146,7 +24146,7 @@
       </c>
       <c r="I386" t="inlineStr">
         <is>
-          <t>roxithromycine,roxithromycinum,roxitromicina,rulide</t>
+          <t/>
         </is>
       </c>
       <c r="J386">
@@ -24210,7 +24210,7 @@
       </c>
       <c r="I387" t="inlineStr">
         <is>
-          <t>rufloxacine,rufloxacinhcl,rufloxacino,rufloxacinum</t>
+          <t>monos,rufloxacine,rufloxacino,rufloxacinum,tebraxin,uroflox</t>
         </is>
       </c>
       <c r="J387">
@@ -24328,7 +24328,7 @@
       </c>
       <c r="I389" t="inlineStr">
         <is>
-          <t>difloxacine,difloxacino,difloxacinum,quinoloneder,saraflox,sarafloxacine,sarafloxacino,sarafloxacinum</t>
+          <t>difloxacino,difloxacinum,difloxcine,sarafin,saraflox,sarafloxacine,sarafloxacino,sarafloxacinum</t>
         </is>
       </c>
       <c r="J389" t="e">
@@ -24390,7 +24390,7 @@
       </c>
       <c r="I390" t="inlineStr">
         <is>
-          <t>seysara</t>
+          <t>sareciclina,seysara</t>
         </is>
       </c>
       <c r="J390">
@@ -24450,7 +24450,7 @@
       </c>
       <c r="I391" t="inlineStr">
         <is>
-          <t/>
+          <t>sarmoxillina,sarmoxilline,sarmoxillinum</t>
         </is>
       </c>
       <c r="J391" t="e">
@@ -24634,7 +24634,7 @@
       </c>
       <c r="I394" t="inlineStr">
         <is>
-          <t>rickamicin,salvamina,siseptinsulfate,sisomicina,sisomicine,sisomicinsulfate,sisomicinum,sisomin,sisomycin,sissomicin,sizomycin</t>
+          <t>rickamicin,salvamina,sisomicina,sisomicine,sisomicinum,sisomin,sisomycin,sissomicin,sizomycin</t>
         </is>
       </c>
       <c r="J394" t="e">
@@ -24694,7 +24694,7 @@
       </c>
       <c r="I395" t="inlineStr">
         <is>
-          <t>gracevit,sitafloxacinisomer</t>
+          <t>gracevit</t>
         </is>
       </c>
       <c r="J395">
@@ -24758,7 +24758,7 @@
       </c>
       <c r="I396" t="inlineStr">
         <is>
-          <t>bactylan,decapasil,lepasen,monopas,nippas,pamisylsodium,parasalsodium,pasade,pasnal,passodico,passodium,salvis,sanipirol,sodiopas,sodiumpas,teebacin,tubersan</t>
+          <t>bactylan,lepasen,monopas,tubersan</t>
         </is>
       </c>
       <c r="J396">
@@ -24882,7 +24882,7 @@
       </c>
       <c r="I398" t="inlineStr">
         <is>
-          <t>esparfloxacino,sparfloxacine,sparfloxacinum</t>
+          <t>esparfloxacino,parox,spara,sparfloxacine,sparfloxacinum,zagam</t>
         </is>
       </c>
       <c r="J398">
@@ -24946,7 +24946,7 @@
       </c>
       <c r="I399" t="inlineStr">
         <is>
-          <t>actinospectacina,adspec,espectinomicina,prospec,specitinomycin,spectam,spectinomicina,spectinomycindihcl,spectinomycine,spectinomycinum,stanilo,togamycin,trobicin</t>
+          <t>actinospectacina,adspec,espectinomicina,prospec,spectam,spectinomicina,spectinomycine,spectinomycinhydrate,spectinomycinum,spectogard,stanilo,togamycin,trobicin</t>
         </is>
       </c>
       <c r="J399" t="e">
@@ -25010,7 +25010,7 @@
       </c>
       <c r="I400" t="inlineStr">
         <is>
-          <t>espiramicin,provamycin,rovamycin,rovamycine,sequamycin,spiramycine,spiramycinum</t>
+          <t>formacidine</t>
         </is>
       </c>
       <c r="J400">
@@ -25136,7 +25136,7 @@
       </c>
       <c r="I402" t="inlineStr">
         <is>
-          <t>ambistrin</t>
+          <t/>
         </is>
       </c>
       <c r="J402" t="e">
@@ -25200,7 +25200,7 @@
       </c>
       <c r="I403" t="inlineStr">
         <is>
-          <t>agrept,agrimycin,chemform,estreptomicina,neodiestreptopab,strepcen,streptomicina,streptomycina,streptomycine,streptomycinspx,streptomycinsulfate,streptomycinum,streptomyzin,vetstrep</t>
+          <t>agrept,agrimycin,chemform,estreptomicina,gerox,neodiestreptopab,strepcen,streptomicina,streptomycine,streptomycinum,streptomyzin</t>
         </is>
       </c>
       <c r="J403" t="e">
@@ -25384,7 +25384,7 @@
       </c>
       <c r="I406" t="inlineStr">
         <is>
-          <t>betamaze,sulbactamacid,sulbactamfreeacid,sulbactamum</t>
+          <t>betamaze,sulbactamum</t>
         </is>
       </c>
       <c r="J406" t="e">
@@ -25448,7 +25448,7 @@
       </c>
       <c r="I407" t="inlineStr">
         <is>
-          <t>kedacillina,sulbenicilina,sulbenicilline,sulbenicillinum</t>
+          <t>kedacillin,kedacillina,sulbenicilina,sulbenicilline,sulbenicillinum,sulpelin</t>
         </is>
       </c>
       <c r="J407" t="e">
@@ -25566,7 +25566,7 @@
       </c>
       <c r="I409" t="inlineStr">
         <is>
-          <t>cluricol,cosulid,cosumix,durasulf,nefrosul,nsulfanilamide,prinzonevet,solfaclorpiridazina,sonilyn,sulfacloropiridazina,vetisulid</t>
+          <t>cluricol,cosulid,cosumix,durasulf,nefrosul,nsulfanilamide,prinzone,solfaclorpiridazina,sonilyn,sulfacloropiridazina,sulfaclorpiridazina,vetisulid</t>
         </is>
       </c>
       <c r="J409" t="e">
@@ -25628,7 +25628,7 @@
       </c>
       <c r="I410" t="inlineStr">
         <is>
-          <t>adiazin,adiazine,cocodiazine,codiazine,cremodiazine,cremotres,debenal,deltazina,diazin,diazolone,diazovit,diazyl,eskadiazine,honeydiazine,liquadiazine,microsulfon,neazine,neotrizine,nsulfanilamide,palatrize,piridisir,pirimal,pyrimal,quadetts,quadramoid,sanodiazine,sildaflo,silvadene,solfadiazina,spofadrizine,sterazine,sulfacombin,sulfadiazene,sulfadiazin,sulfadiazina,sulfadiazinum,sulfapirimidin,sulfapyrimidin,sulfapyrimidine,sulfatryl,sulfazine,sulfolex,sulfonamidesduplex,sulfonsol,sulfose,sulphadiazine,sulphadiazinee,terfonyl,theradiazine,thermazene,trifonamide,triplesulfa,triplesulfas,trisem,truozine,zincsulfadiazine</t>
+          <t>adiazin,adiazine,codiazine,cremodiazine,cremotres,debenal,deltazina,dermazin,dermazine,diazin,diazolone,diazovit,eskadiazine,flamazine,geben,liquadiazine,microsulfon,neazine,neotrizine,palatrize,piridisir,pirimal,pyrimal,quadetts,quadramoid,sanodiazine,silbertone,sildaflo,silvadene,silvazine,silver,silveramide,sliverex,solfadiazina,spofadrizine,sterazine,sulfacombin,sulfadiazene,sulfadiazin,sulfadiazina,sulfadiazinum,sulfapirimidin,sulfapyrimidin,sulfapyrimidine,sulfatryl,sulfazine,sulfolex,sulfonsol,sulfose,sulphadiazine,terfonyl,theradiazine,thermazene,trifonamide,trisem,truozine</t>
         </is>
       </c>
       <c r="J410">
@@ -25692,7 +25692,7 @@
       </c>
       <c r="I411" t="inlineStr">
         <is>
-          <t>cotetroxazine</t>
+          <t>berlocombin,cotetroxazine,potesept,trimerazine</t>
         </is>
       </c>
       <c r="J411" t="e">
@@ -25754,7 +25754,7 @@
       </c>
       <c r="I412" t="inlineStr">
         <is>
-          <t>antastmon,cotrimazine,diaziprimforte,ditrim,ditrivet,sultrisan,triglobe,trimin,tucoprim,uniprim</t>
+          <t>antastmon,astra,ditrim,ditrivet,sultrisan,triglobe,trimin,tucoprim,uniprim</t>
         </is>
       </c>
       <c r="J412" t="e">
@@ -25816,7 +25816,7 @@
       </c>
       <c r="I413" t="inlineStr">
         <is>
-          <t>agribon,arnosulfan,bactrovet,deposul,diasulfa,diasulfyl,dimetazina,dinosol,dorisul,lasibon,madribon,madrigid,madriqid,madroxin,madroxine,maxulvet,mecozine,memcozine,metoxidon,neostrepal,neostreptal,nsulfanilamide,omnibon,persulfen,primor,radonin,redifal,rofenaid,roscosulf,scandisil,solfadimetossina,sudine,suldixine,sulfabon,sulfadimethoxin,sulfadimethoxinum,sulfadimetossina,sulfadimetoxin,sulfadimetoxina,sulfadimetoxine,sulfadimoxine,sulfastop,sulfdimethoxine,sulfoplan,sulphadimethoxine,sulxin,sumbio,symbio,theracanzan,ultrasulfon</t>
+          <t>abcid,agribon,albon,arnosulfan,bactotril,bactrovet,deposul,diasulfa,diasulfyl,dimetazina,dinosol,dorisul,fuxal,lasibon,madribon,madrigid,madriqid,madroxin,madroxine,maxulvet,mecozine,memcozine,metoxidon,neostrepal,neostreptal,nsulfanilamidesalt,omnibon,persulfen,radonin,redifal,rofenaid,roscosulf,scandisil,solfadimetossina,sudine,suldixine,sulfabon,sulfadimethoxin,sulfadimethoxinesalt,sulfadimethoxinum,sulfadimetossina,sulfadimetoxin,sulfadimetoxina,sulfadimetoxine,sulfadimoxine,sulfastop,sulfoplan,sulforal,sulphadimethoxine,sulxin,sumbio,symbio,theracanzan,ultrasulfon</t>
         </is>
       </c>
       <c r="J413">
@@ -25880,7 +25880,7 @@
       </c>
       <c r="I414" t="inlineStr">
         <is>
-          <t>azolmetazin,benzenesulfonamide,calfspan,calfspantablets,cremomethazine,diazil,diazilsulfadine,dimezathine,intradine,kelametazine,mermeth,metazin,neasina,neazina,nsulfanilamide,panazin,pirmazin,primazin,saiii,solfadimidina,spanbolet,sulfadimerazine,sulfadimesin,sulfadimesine,sulfadimethyldiazine,sulfadimezin,sulfadimezine,sulfadimezinum,sulfadimidin,sulfadimidina,sulfadimidinum,sulfadine,sulfametazina,sulfametazyny,sulfamethiazine,sulfamezathine,sulfamidine,sulfasuresrbolus,sulfodimesin,sulfodimezine,sulkakboluses,sulkasboluses,sulmet,sulphadimidine,sulphamethasine,sulphamethazine,sulphamezathine,sulphamidine,sulphodimezine,superseptil,superseptyl,vertolan</t>
+          <t>azolmetazin,bovibol,calfspan,cremomethazine,diazil,diazilsulfadine,diazyl,dimezathine,intradine,kelametazine,mermeth,neasina,neazina,panazin,pirmazin,primazin,solfadimidina,spanbolet,sulfadimerazine,sulfadimesin,sulfadimesine,sulfadimethyldiazine,sulfadimezin,sulfadimezine,sulfadimezinum,sulfadimidin,sulfadimidina,sulfadimidinum,sulfadimidinun,sulfadine,sulfametazina,sulfametazyny,sulfamethiazine,sulfamezathine,sulfamidine,sulfodimesin,sulfodimezine,sulmet,sulphadimidine,sulphamethasine,sulphamethazine,sulphamezathine,sulphamidine,sulphodimezine,superseptil,superseptyl,vertolan,vesadin</t>
         </is>
       </c>
       <c r="J414">
@@ -26006,7 +26006,7 @@
       </c>
       <c r="I416" t="inlineStr">
         <is>
-          <t>accuzole,alphazole,amidoxal,astrazolo,azogantrisin,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,dorsulfanwarthausen,entusil,entusul,eryzole,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazoi,neoxazol,novazolo,novosaxazole,nsulfanilamide,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxosultablets,roxoxol,saxosozine,sodizole,solfafurazolo,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafurazol,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan,vagilia</t>
+          <t>accuzole,alphazole,amidoxal,astrazolo,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,entusil,entusul,ganda,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazol,novazolo,novosaxazole,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxoxol,saxosozine,sodizole,solfafurazolo,sosol,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafurazol,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan</t>
         </is>
       </c>
       <c r="J416">
@@ -26072,7 +26072,7 @@
       </c>
       <c r="I417" t="inlineStr">
         <is>
-          <t>aristamid,aristamide,aristogyn,domain,domian,elcosin,elcosine,elkosil,elkosin,elkosine,erycon,isosulf,mefenal,nsulfanilamide,solfisomidina,sulfadimetine,sulfaisodimerazine,sulfaisodimidinum,sulfaisomidine,sulfamethin,sulfasomidine,sulfisomidina,sulfisomidine,sulfisomidinesodium,sulfisomidinum,sulphasomidine</t>
+          <t>aristamid,aristamide,aristogyn,domain,domian,elcosin,elcosine,elkosil,elkosin,elkosine,erycon,isosulf,mefenal,solfisomidina,sulfadimetine,sulfaisodimerazine,sulfaisodimidinum,sulfaisomidine,sulfasomidine,sulfisomidin,sulfisomidina,sulfisomidine,sulfisomidinum,sulphasomidine</t>
         </is>
       </c>
       <c r="J417">
@@ -26138,7 +26138,7 @@
       </c>
       <c r="I418" t="inlineStr">
         <is>
-          <t>dalysep,kelfizin,kelfizina,kelfizine,kelfizinew,longum,nsulfanilamide,policydal,polycidal,solfametopirazina,sulfalen,sulfaleno,sulfalenum,sulfamethopyrazine,sulfamethoxypyrazine,sulfametopyrazine,sulfametoxypyridazin,sulphalene,sulphametopyrazine,vetkelfizina</t>
+          <t>dalysep,farmitalia,kelfizin,kelfizina,kelfizine,policydal,solfametopirazina,sulfalen,sulfaleno,sulfalenum,sulfamethopyrazine,sulfamethoxypyrazine,sulfametopyrazine,sulfametoxypyridazin,sulphalene,sulphametopyrazine,vetkelfizina</t>
         </is>
       </c>
       <c r="J418">
@@ -26202,7 +26202,7 @@
       </c>
       <c r="I419" t="inlineStr">
         <is>
-          <t>sulfamazon,sulfamazona,sulfamazonum</t>
+          <t>sulfamazona,sulfamazonum,sulfenazone</t>
         </is>
       </c>
       <c r="J419">
@@ -26266,7 +26266,7 @@
       </c>
       <c r="I420" t="inlineStr">
         <is>
-          <t>cremomerazine,kelamerazine,mebacid,mesulfa,methylpyrimal,methylsulfazin,methylsulfazine,metilsulfadiazin,metilsulfazin,nsulfanilamide,percoccide,pyralcid,pyrimalm,romezin,septacil,septosyl,solfamerazina,solumedin,solumedine,sulfameradine,sulfamerazin,sulfamerazina,sulfamerazinum,sulfamethyldiazine,sulphamerazine,sumedine,susfamerazine</t>
+          <t>cremomerazine,kelamerazine,mebacid,mesulfa,methylpyrimal,methylsulfazin,methylsulfazine,metilsulfadiazin,metilsulfazin,percoccide,pyralcid,romezin,septacil,septosyl,solfamerazina,solumedin,solumedine,sulfameradine,sulfamerazin,sulfamerazina,sulfamerazinum,sulfamethyldiazine,sulphamerazine,sumedine</t>
         </is>
       </c>
       <c r="J420">
@@ -26388,7 +26388,7 @@
       </c>
       <c r="I422" t="inlineStr">
         <is>
-          <t>azolmetazin,benzenesulfonamide,calfspan,calfspantablets,cremomethazine,diazil,diazilsulfadine,dimezathine,intradine,kelametazine,mermeth,metazin,neasina,neazina,nsulfanilamide,panazin,pirmazin,primazin,saiii,solfadimidina,spanbolet,sulfadimerazine,sulfadimesin,sulfadimesine,sulfadimethyldiazine,sulfadimezin,sulfadimezine,sulfadimezinum,sulfadimidin,sulfadimidina,sulfadimidinum,sulfadine,sulfametazina,sulfametazyny,sulfamethiazine,sulfamezathine,sulfamidine,sulfasuresrbolus,sulfodimesin,sulfodimezine,sulkakboluses,sulkasboluses,sulmet,sulphadimidine,sulphamethasine,sulphamethazine,sulphamezathine,sulphamidine,sulphodimezine,superseptil,superseptyl,vertolan</t>
+          <t/>
         </is>
       </c>
       <c r="J422" t="e">
@@ -26450,7 +26450,7 @@
       </c>
       <c r="I423" t="inlineStr">
         <is>
-          <t>ayerlucil,lucosil,methazol,microsul,nsulfanilamide,proklar,renasul,salimol,solfametizolo,sulamethizole,sulfagram,sulfamethizol,sulfamethizolum,sulfametizol,sulfapyelon,sulfstat,sulfurine,sulphamethizole,tetracid,thidicur,thiosulfil,thiosulfilforte,ultrasul,urocydal,urodiaton,urolucosil,urosulfin</t>
+          <t>aethazol,aethazolum,ayerlucil,berlophen,etazol,etazole,ethazole,famet,gliprotiazol,globucid,globucin,globuzid,glyprothiazol,glyprothiazole,glyprothiazolum,glyprothizolum,lucosil,methazol,microsul,proklar,renasul,rufol,salimol,sethadil,solfametizolo,solfetidolo,sulfaethidiole,sulfaethidol,sulfaethidole,sulfaethidolum,sulfaetidol,sulfamethizol,sulfamethizolum,sulfametizol,sulfapyelon,sulfstat,sulfurine,sulphaethidole,sulphamethizole,tardipyrine,tetracid,thidicur,thiosulfil,ultrasul,urocydal,urodiaton,urolucosil,urosulfin</t>
         </is>
       </c>
       <c r="J423">
@@ -26514,7 +26514,7 @@
       </c>
       <c r="I424" t="inlineStr">
         <is>
-          <t>azogantanol,gamazole,gantanol,gantanolds,metoxal,nsulfanilamide,nsulphanilamide,radonil,septran,simsinomin,sinomin,solfametossazolo,sulfamethalazole,sulfamethoxazol,sulfamethoxazolum,sulfamethoxizole,sulfamethylisoxazole,sulfametoxazol,sulfisomezole,sulmeprim,sulphamethalazole,sulphamethoxazol,sulphamethoxazole,sulphisomezole,urobak</t>
+          <t>septran,septrin,simsinomin,sinomin,solfametossazolo,sulfamethalazole,sulfamethoxazol,sulfamethoxazolum,sulfamethoxizole,sulfamethylisoxazole,sulfametoxazol,sulfiodizole,sulfisomezole,sulphamethoxazol,sulphamethoxazole,sulphisomezole,urobak</t>
         </is>
       </c>
       <c r="J424">
@@ -26578,7 +26578,7 @@
       </c>
       <c r="I425" t="inlineStr">
         <is>
-          <t>altezol,davosin,depovernil,kineks,lederkyn,lentac,lisulfen,longin,medicel,midicel,midikel,myasul,nsulfanilamide,opinsul,paramid,paramidsupra,petrisul,piridolo,quinoseptyl,retamid,retasulfin,retasulphine,slosul,spofadazine,sulfalex,sulfapyridazine,sulfdurazin,sulfozona,sultirene,vinces</t>
+          <t>altezol,cysul,davosin,depovernil,durox,kineks,kinex,kynex,lederkyn,lentac,lisulfen,longin,medicel,midicel,midikel,myasul,opinsul,paramid,petrisul,piridolo,quinoseptyl,retamid,retasulfin,retasulphine,slosul,spofadazine,succinylsulfathi,sulfalex,sulfapiridazin,sulfapyridazine,sulfdurazin,sulfozona,sultirene,vinces</t>
         </is>
       </c>
       <c r="J425">
@@ -26642,7 +26642,7 @@
       </c>
       <c r="I426" t="inlineStr">
         <is>
-          <t>duroprocin,methofadin,methofazine,nsulfanilamide,solfametomidina,sulfamethomidine,sulfametomidin,sulfametomidina,sulfametomidinum</t>
+          <t>duroprocin,methofadin,methofazine,solfametomidina,sulfametomidin,sulfametomidina,sulfametomidinum,telemid</t>
         </is>
       </c>
       <c r="J426" t="e">
@@ -26704,7 +26704,7 @@
       </c>
       <c r="I427" t="inlineStr">
         <is>
-          <t>bayrena,berlicid,dairena,durenat,juvoxin,kinecid,kirocid,longasulf,methoxypyrimal,nsulfanilamide,solfametossidiazina,sulfameter,sulfamethorine,sulfamethoxine,sulfamethoxydiazin,sulfamethoxydiazine,sulfamethoxydin,sulfamethoxydine,sulfametin,sulfametinum,sulfametorin,sulfametorine,sulfametorinum,sulfametoxidiazina,sulfametoxidine,sulfametoxydiazinum,sulphameter,sulphamethoxydiazine,supramid,ultrax</t>
+          <t>bayrena,berlicid,dairena,durenat,juvoxin,kinecid,kirocid,kiron,longasulf,methoxypyrimal,solfametossidiazina,sulfameter,sulfametersalt,sulfamethorine,sulfamethoxine,sulfamethoxydiazin,sulfamethoxydiazine,sulfamethoxydin,sulfamethoxydine,sulfametin,sulfametinum,sulfametorine,sulfametorinum,sulfametoxidiazina,sulfametoxidine,sulfametoxydiazinum,sulla,sulphameter,sulphamethoxydiazine,supramid,ultrax</t>
         </is>
       </c>
       <c r="J427">
@@ -26830,7 +26830,7 @@
       </c>
       <c r="I429" t="inlineStr">
         <is>
-          <t>justamil,nsulfanilamide,oxasulfa,solfamossolo,sulfadimethyloxazole,sulfamoxol,sulfamoxolum,sulfano,sulfavigor,sulfmidil,sulfono,sulfune,sulfuno,sulphamoxole,tardamid,tardamide</t>
+          <t>enterocura,justamil,oxasulfa,solfaguanolo,solfamossolo,sulfadimethyloxazole,sulfaguanol,sulfaguanole,sulfaguanolum,sulfamoxol,sulfamoxolum,sulfano,sulfavigor,sulfmidil,sulfono,sulfune,sulfuno,sulphamoxole,tardamid,tardamide</t>
         </is>
       </c>
       <c r="J429">
@@ -26896,7 +26896,7 @@
       </c>
       <c r="I430" t="inlineStr">
         <is>
-          <t>cotrifamole</t>
+          <t/>
         </is>
       </c>
       <c r="J430" t="e">
@@ -26958,7 +26958,7 @@
       </c>
       <c r="I431" t="inlineStr">
         <is>
-          <t>albexan,albosal,ambeside,antistrept,astreptine,astrocid,bacteramid,bactesid,collomide,colsulanyde,copticide,deseptyl,desseptyl,dipron,ergaseptine,erysipan,estreptocida,exoseptoplix,gerison,gombardol,infepan,lysococcine,neococcyl,orgaseptine,prontalbin,prontosilalbum,prontosili,prontosilwhite,prontylin,pronzinalbum,proseptal,proseptine,proseptol,pysococcine,rubiazola,sanamid,septamidealbum,septanilam,septinal,septolix,septoplex,septoplix,solfanilamide,stoptonalbum,stramid,strepamide,strepsan,streptagol,streptamid,streptamin,streptasol,streptocid,streptocidalbum,streptocide,streptocidewhite,streptocidum,streptoclase,streptocom,streptol,strepton,streptopan,streptosil,streptozol,streptozone,streptrocide,sulfamidyl,sulfamine,sulfana,sulfanalone,sulfanidyl,sulfanil,sulfanilamida,sulfanilamidum,sulfanilimidicacid,sulfanimide,sulfocidin,sulfocidine,sulfonamidep,sulfonylamide,sulphanilamide,sulphanilamidegr,sulphanilamidum,sulphonamide,therapol,tolder,whitestreptocide</t>
+          <t>albexan,albosal,ambeside,antistrept,astreptine,astrocid,bacteramid,bactesid,collomide,colsulanyde,copticide,deseptyl,dipron,ergaseptine,erysipan,estreptocida,exoseptoplix,fourneau,gerison,gombardol,hydroxysulfonamide,infepan,lusil,lysococcine,neococcyl,orgaseptine,prontalbin,prontylin,proseptal,proseptine,proseptol,pysococcine,sanamid,septanilam,septinal,septolix,septoplex,septoplix,solfanilamide,stramid,strepamide,strepsan,streptagol,streptamid,streptamin,streptasol,streptocid,streptocide,streptocidum,streptoclase,streptocom,strepton,streptopan,streptosil,streptozol,streptozone,streptrocide,sulfamidyl,sulfamine,sulfana,sulfanalone,sulfanidyl,sulfanil,sulfanilamida,sulfanilamidomethan,sulfanilamidum,sulfanimide,sulfocidin,sulfocidine,sulfonylamide,sulphanilamide,sulphanilamidum,sulphonamide,therapol,tolder</t>
         </is>
       </c>
       <c r="J431" t="e">
@@ -27020,7 +27020,7 @@
       </c>
       <c r="I432" t="inlineStr">
         <is>
-          <t>anastaf,archisulfa,avissul,chemiopen,demosulfan,durisansaft,ipersulfidinsirup,isosulfamerazine,methylsulfadiazin,methylsulfadiazine,novosul,nsulfanilamide,orosulfan,pallidin,retardon,risulfasens,sulfaperina,sulfaperine,sulfaperinum,sulfatreis,sulfopirimidine,sulpenta,ultrasulfonsirup</t>
+          <t>anastaf,archisulfa,archisulpha,avissul,chemiopen,demosulfan,demosulphan,durisan,isosulfamerazine,isosulphamerazine,methylsulfadiazin,methylsulfadiazine,methylsulphadiazine,novosul,orosulfan,pallidin,retardon,risulfasens,sulfaperina,sulfaperine,sulfaperinum,sulfatreis,sulfopirimidine,sulpenta,sulphaperin,sulphaperina,sulphaperinum</t>
         </is>
       </c>
       <c r="J432">
@@ -27084,7 +27084,7 @@
       </c>
       <c r="I433" t="inlineStr">
         <is>
-          <t>depocid,depotsulfonamide,eftolon,firmazolo,inamil,isarol,isarolv,merian,microtanpirazolo,nsulfanilamide,orisul,orisulf,paidazolo,phenylsulfapyrazole,plisulfan,raziosulfa,solfafenazolo,sulfabid,sulfafenazol,sulfafenazolo,sulfaphenazol,sulfaphenazolum,sulfaphenazon,sulfaphenylpipazol,sulfaphenylpyrazol,sulfaphenylpyrazole,sulfonylpyrazol,sulphaphenazole,sulphenazole</t>
+          <t>depocid,depotsulfonamide,eftolon,firmazolo,inamil,isarol,merian,orisul,orisulf,paidazolo,phenylsulfapyrazole,plisulfan,raziosulfa,solfafenazolo,sulfabid,sulfafenazol,sulfafenazolo,sulfaphenazol,sulfaphenazolum,sulfaphenazon,sulfaphenylpipazol,sulfaphenylpyrazol,sulfaphenylpyrazole,sulfonylpyrazol,sulphaphenazole,sulphenazole</t>
         </is>
       </c>
       <c r="J433">
@@ -27148,7 +27148,7 @@
       </c>
       <c r="I434" t="inlineStr">
         <is>
-          <t>adiplon,coccoclase,dagenan,eubasin,eubasinum,haptocil,piridazol,plurazol,pyriamid,pyridazol,relbapiridina,septipulmon,solfapiridina,streptosilpyridine,sulfapiridina,sulfapyridin,sulfapyridinum,sulfidin,sulfidine,sulphapyridin,sulphapyridine,thioseptal,trianon</t>
+          <t>adiplon,coccoclase,dagenan,eubasin,eubasinum,haptocil,piridazol,plurazol,pyriamid,pyridazol,relbapiridina,ronin,septipulmon,solfapiridina,soludagenan,streptosilpyridine,sulfapiridina,sulfapyridin,sulfapyridinum,sulfidin,sulfidine,sulphapyridin,sulphapyridine,thioseptal,trianon</t>
         </is>
       </c>
       <c r="J434">
@@ -27208,7 +27208,7 @@
       </c>
       <c r="I435" t="inlineStr">
         <is>
-          <t>ambesid,derganil,sulfasuccinamid,sulfasuccinamida,sulfasuccinamidum</t>
+          <t>sulfasuccinamid,sulfasuccinamida,sulfasuccinamidum</t>
         </is>
       </c>
       <c r="J435" t="e">
@@ -27270,7 +27270,7 @@
       </c>
       <c r="I436" t="inlineStr">
         <is>
-          <t>azoquimiol,azoseptale,cerazol,cerazole,chemosept,cibazol,duatok,dulana,eleudron,enterobiocine,estafilol,formosulfathiazole,neostrepsan,norsulfasol,norsulfazol,norsulfazole,norsulfazolum,nsulfanilamide,planomide,poliseptil,sanotiazol,septozol,sodiumsulfathiazole,solfatiazolo,streptosilthiazole,sulfamul,sulfathiazol,sulfathiazolum,sulfatiazol,sulfavitina,sulfocerol,sulphathiazole,sulzol,thiacoccine,thiasulfol,thiazamide,thiozamide,triplesulfa,wintrazole</t>
+          <t>azoquimiol,azoseptale,cerazol,cerazole,chemosept,cibazol,duatok,dulana,eleudron,enterobiocine,estafilol,formosulfathiazole,neostrepsan,norsulfasol,norsulfazol,norsulfazole,norsulfazolum,planomide,poliseptil,sanotiazol,septozol,solfatiazolo,soluthiazomide,streptosilthiazole,sulfamul,sulfaplex,sulfathiazol,sulfathiazolesalt,sulfathiazolum,sulfatiazol,sulfavitina,sulfocerol,sulphathiazole,sulzol,thiacoccine,thiasulfol,thiazamide,thiozamide,wintrazole</t>
         </is>
       </c>
       <c r="J436" t="e">
@@ -27332,7 +27332,7 @@
       </c>
       <c r="I437" t="inlineStr">
         <is>
-          <t>badional,baldinol,fontamide,salvoseptyl,solfatiourea,solufontamide,sulfanilthiourea,sulfathiocarbamid,sulfathiocarbamide,sulfathiocarbamidum,sulfathiouree,sulfatiourea,sulphathiourea</t>
+          <t>badional,baldinol,fontamide,salvoseptyl,solfatiourea,solufontamide,sulfanilthiourea,sulfathiocarbamid,sulfathiocarbamide,sulfathiocarbamidum,sulfathioureasalt,sulfathiouree,sulfatiourea,sulphathiourea</t>
         </is>
       </c>
       <c r="J437">
@@ -27392,7 +27392,7 @@
       </c>
       <c r="I438" t="inlineStr">
         <is>
-          <t>accuzole,alphazole,amidoxal,astrazolo,azogantrisin,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,dorsulfanwarthausen,entusil,entusul,eryzole,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazoi,neoxazol,novazolo,novosaxazole,nsulfanilamide,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxosultablets,roxoxol,saxosozine,sodizole,solfafurazolo,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafurazol,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan,vagilia</t>
+          <t/>
         </is>
       </c>
       <c r="J438" t="e">
@@ -27450,7 +27450,7 @@
       </c>
       <c r="I439" t="inlineStr">
         <is>
-          <t>anhydron,aquirel,ciclotiazida,ciclotiazide,cyclothiazide,cyclothiazidum,doburil,fluidil,renazide,valmiran</t>
+          <t/>
         </is>
       </c>
       <c r="J439" t="e">
@@ -27508,7 +27508,7 @@
       </c>
       <c r="I440" t="inlineStr">
         <is>
-          <t/>
+          <t>orlynvah</t>
         </is>
       </c>
       <c r="J440" t="e">
@@ -27570,7 +27570,7 @@
       </c>
       <c r="I441" t="inlineStr">
         <is>
-          <t>sultamicilina,sultamicillinum</t>
+          <t>combisid,sultamicilina,sultamicilline,sultamicillinum,unacid</t>
         </is>
       </c>
       <c r="J441">
@@ -27630,7 +27630,7 @@
       </c>
       <c r="I442" t="inlineStr">
         <is>
-          <t/>
+          <t>surotomicina,surotomycine</t>
         </is>
       </c>
       <c r="J442" t="e">
@@ -27692,7 +27692,7 @@
       </c>
       <c r="I443" t="inlineStr">
         <is>
-          <t>talampicilina,talampicilline,talampicillinum</t>
+          <t>aseocillin,phthalidyl,talampicilina,talampicilline,talampicillinum,talpen,yamacillin</t>
         </is>
       </c>
       <c r="J443">
@@ -27814,7 +27814,7 @@
       </c>
       <c r="I445" t="inlineStr">
         <is>
-          <t>tazobactamacid,tazobactamum,tazobactum</t>
+          <t>enmetazobactam,exblifep,tazobactamsalt,tazobactamum,tazobactum</t>
         </is>
       </c>
       <c r="J445" t="e">
@@ -27872,7 +27872,7 @@
       </c>
       <c r="I446" t="inlineStr">
         <is>
-          <t>tebipenempivoxil</t>
+          <t/>
         </is>
       </c>
       <c r="J446">
@@ -27936,7 +27936,7 @@
       </c>
       <c r="I447" t="inlineStr">
         <is>
-          <t>sivextro,torezolid</t>
+          <t>torezolid</t>
         </is>
       </c>
       <c r="J447">
@@ -28002,7 +28002,7 @@
       </c>
       <c r="I448" t="inlineStr">
         <is>
-          <t>targocid,tecoplanina,tecoplanine,tecoplaninum,teichomycin,teicoplanina,teicoplanine,teicoplaninum</t>
+          <t/>
         </is>
       </c>
       <c r="J448" t="e">
@@ -28124,7 +28124,7 @@
       </c>
       <c r="I450" t="inlineStr">
         <is>
-          <t>televancin,vibativ</t>
+          <t>arbelic,nvancomycin,televancin</t>
         </is>
       </c>
       <c r="J450" t="e">
@@ -28186,7 +28186,7 @@
       </c>
       <c r="I451" t="inlineStr">
         <is>
-          <t>levviax</t>
+          <t>ketek,levviax</t>
         </is>
       </c>
       <c r="J451">
@@ -28250,7 +28250,7 @@
       </c>
       <c r="I452" t="inlineStr">
         <is>
-          <t>omniflox,temafloxacina,temafloxacine,temafloxacinum</t>
+          <t>omniflox,temafloxacina,temafloxacine,temafloxacino,temafloxacinum</t>
         </is>
       </c>
       <c r="J452">
@@ -28378,7 +28378,7 @@
       </c>
       <c r="I454" t="inlineStr">
         <is>
-          <t>corbinal,lamasil,lamisil,lamisilat,lamisiltablet,terbinafina,terbinafinum,terbinex</t>
+          <t>afogan,bramazil,bramizil,corbinal,lamasil,lamisil,muzonal,shoprite,terbina,terbinafina,terbinafinum,terbine,terbinex,terbisil,zabel</t>
         </is>
       </c>
       <c r="J454">
@@ -28438,7 +28438,7 @@
       </c>
       <c r="I455" t="inlineStr">
         <is>
-          <t>fungistat,panlomyc,terazol,terconazol,terconazolum,tercospor,triaconazole,zazole</t>
+          <t>fungistat,panlomyc,terazol,terconazol,terconazolum,tercospor,tetrazol,triaconazole,zazole</t>
         </is>
       </c>
       <c r="J455" t="e">
@@ -28500,7 +28500,7 @@
       </c>
       <c r="I456" t="inlineStr">
         <is>
-          <t>terivalidin,terizidon,terizidona,terizidonum</t>
+          <t>terivalidin,terizidona,terizidonum</t>
         </is>
       </c>
       <c r="J456" t="e">
@@ -28562,7 +28562,7 @@
       </c>
       <c r="I457" t="inlineStr">
         <is>
-          <t>abramycin,abricycline,achromycin,achromycinv,actisite,agromicina,ambramicina,ambramycin,amycin,biocycline,bristaciclin,bristaciclina,bristacycline,brodspec,cefracycline,centet,ciclibion,copharlan,criseociclina,cyclomycin,cyclopar,cytome,democracin,deschlorobiomycin,dumocyclin,economycin,enterocycline,hostacyclin,lexacycline,limecycline,liquamycin,medocycline,mericycline,micycline,neocycline,oletetrin,omegamycin,orlycycline,panmycin,piracaps,polycycline,polyotic,purocyclina,resteclin,robitet,roviciclina,sigmamycin,solvocin,sumycin,sumycinsyrup,supramycin,sustamycin,tetrabidorganon,tetrabon,tetrachel,tetraciclina,tetracycl,tetracyclin,tetracyclinebase,tetracyclinehydrate,tetracyclinei,tetracyclineii,tetracyclinum,tetracyn,tetradecin,tetrafil,tetramed,tetrasure,tetraverine,tetrazyklin,tetrex,topicycline,tsiklomistsin,tsiklomitsin,veracin,vetacyclinum,vetquamycin</t>
+          <t>abramycin,abricycline,agromicina,ambramicina,ambramycin,amycin,biocycline,brodspec,cefracycline,centet,ciclibion,copharlan,criseociclina,cyclomycin,democracin,deschlorobiomycin,economycin,hostacyclin,lexacycline,limecycline,liquamycin,mericycline,micycline,neocycline,omegamycin,orlycycline,panmycin,purocyclina,roviciclina,solvocin,tetrabon,tetraciclina,tetracycl,tetracyclin,tetracyclinehydrate,tetracyclinum,tetracyn,tetradecin,tetrafil,tetraverine,tetrazyklin,tsiklomistsin,tsiklomitsin,veracin,vetacyclinum</t>
         </is>
       </c>
       <c r="J457">
@@ -28744,7 +28744,7 @@
       </c>
       <c r="I460" t="inlineStr">
         <is>
-          <t>tetroxoprima,tetroxoprime,tetroxoprimum</t>
+          <t>primsol,tetroxoprima,tetroxoprime,tetroxoprimum,trimpex,trimplex</t>
         </is>
       </c>
       <c r="J460" t="e">
@@ -28802,7 +28802,7 @@
       </c>
       <c r="I461" t="inlineStr">
         <is>
-          <t>aktivan,ambathizon,amithiozone,amithizone,amitiozon,benthiozone,benzothiozane,benzothiozon,berculona,berkazon,citazone,conteben,diasan,diazan,domakol,ilbion,livazone,mirizoneneustab,mivizon,myvizone,neotibil,neustab,novakol,nuclonargentinian,panrone,parazone,seroden,siocarbazone,tebalon,tebecure,tebemar,tebesonei,tebethion,tebethione,tebezon,thiacetone,thiacetozone,thibon,thibone,thioacetazon,thioacetazonum,thioazetazone,thiocarbazil,thiomicid,thionicid,thioparamizon,thioparamizone,thiosemicarbarzone,thiosemicarbazone,thiotebesin,thiotebezin,thiotebicina,thizone,tiacetazon,tibicur,tibion,tibione,tibizan,tibone,tioacetazon,tioacetazona,tioatsetazon,tiobicina,tiocarone,tiosecolo,tubercazon,tubigal</t>
+          <t>acetanilide,aktivan,ambathizon,amitiozon,antib,benthiozone,benzothiozane,benzothiozon,berkazon,citazone,conteben,diasan,domakol,ilbion,livazone,mivizon,myvizone,neotibil,neustab,novakol,panrone,parazone,seroden,siocarbazone,tebalon,tebecure,tebemar,tebethion,tebethione,tebezon,thiacetone,thiacetozone,thibon,thibone,thioacetazon,thioacetazonum,thioazetazone,thiocarbazil,thiomicid,thionicid,thioparamizon,thioparamizone,thiosemicarbarzone,thiosemicarbazone,thiotebesin,thiotebezin,thiotebicina,thizone,tiacetazon,tibicur,tibion,tibione,tibizan,tibon,tibone,tioacetazon,tioacetazona,tioatsetazon,tiobicina,tiocarone,tiosecolo,tubercazon,tubigal,tubin</t>
         </is>
       </c>
       <c r="J461" t="e">
@@ -28864,7 +28864,7 @@
       </c>
       <c r="I462" t="inlineStr">
         <is>
-          <t>descocin,dexawin,dextrosulfenidol,dextrosulphenidol,efnicol,hyrazin,igralin,macphenicol,masatirin,neomyson,racefenicol,racefenicolo,racefenicolum,raceophenidol,racephenicol,rincrol,thiamcol,thiamphenicolum,thiocymetin,thiomycetin,thiophenicol,tiamfenicol,tiamfenicolo,urfamicina,urfamycine,vicemycetin</t>
+          <t>armai,dextrosulfenidol,dextrosulphenidol,igralin,racefenicol,racefenicolo,racefenicolum,raceophenidol,thiamphenicolum,thiocymetin,thiophenicol,tiamfenicol,tiamfenicolo,urfamycine</t>
         </is>
       </c>
       <c r="J462">
@@ -28930,7 +28930,7 @@
       </c>
       <c r="I463" t="inlineStr">
         <is>
-          <t>aktivan,ambathizon,amithiozone,amitiozon,benthiozone,benzothiozane,benzothiozon,berculona,berkazon,citazone,conteben,diasan,domakol,ilbion,livazone,mirizoneneustab,mivizon,myvizone,neotibil,neustab,novakol,nuclonargentinian,panrone,parazone,seroden,siocarbazone,tebalon,tebecure,tebemar,tebesonei,tebethion,tebethione,tebezon,thiacetone,thiacetozone,thibon,thibone,thioacetazon,thioacetazonum,thioazetazone,thiocarbazil,thiomicid,thionicid,thioparamizon,thioparamizone,thiosemicarbarzone,thiosemicarbazone,thiotebesin,thiotebezin,thiotebicina,thizone,tiacetazon,tibicur,tibion,tibione,tibizan,tibone,tioacetazon,tioacetazona,tioatsetazon,tiobicina,tiocarone,tiosecolo,tubercazon,tubigal</t>
+          <t/>
         </is>
       </c>
       <c r="J463" t="e">
@@ -29050,7 +29050,7 @@
       </c>
       <c r="I465" t="inlineStr">
         <is>
-          <t>denagard,thiamutilin,tiamulina,tiamuline,tiamulinpamoate,tiamulinum,tiavetp</t>
+          <t>denagard,thiamutilin,tiamulina,tiamuline,tiamulinum</t>
         </is>
       </c>
       <c r="J465" t="e">
@@ -29112,7 +29112,7 @@
       </c>
       <c r="I466" t="inlineStr">
         <is>
-          <t>ticarcilina,ticarcilline,ticarcillinum,ticillin,timentin</t>
+          <t>ticar,ticarcilina,ticarcilline,ticarcillinum,ticillin,timentin</t>
         </is>
       </c>
       <c r="J466" t="e">
@@ -29176,7 +29176,7 @@
       </c>
       <c r="I467" t="inlineStr">
         <is>
-          <t>timentin</t>
+          <t>augpenin</t>
         </is>
       </c>
       <c r="J467" t="e">
@@ -29240,7 +29240,7 @@
       </c>
       <c r="I468" t="inlineStr">
         <is>
-          <t>haizhenglixing,tigeciclina,tigecyclin,tigecyclinehydrate,tigecyclinum,tigilcycline,tygacil</t>
+          <t>tigeciclina,tigecyclin,tigecyclinehydrate,tigilcycline,tygacil</t>
         </is>
       </c>
       <c r="J468" t="e">
@@ -29474,7 +29474,7 @@
       </c>
       <c r="I472" t="inlineStr">
         <is>
-          <t>micotil,pulmotil,tilmicosina,tilmicosine,tilmicosinum</t>
+          <t>micotil,pulmotil,tilmicosina,tilmicosine,tilmicosinum,tilmovet</t>
         </is>
       </c>
       <c r="J472" t="e">
@@ -29536,7 +29536,7 @@
       </c>
       <c r="I473" t="inlineStr">
         <is>
-          <t>amtiba,bioshik,ethylsulfone,fasigin,fasigyn,fasigyntrademark,fasygin,glongyn,haisigyn,pletil,simplotan,simplotantrademark,sorquetan,symplotan,tindamax,tindamaxtrademark,tinidazol,tinidazolum,tricolam,trimonase</t>
+          <t>amtiba,bioshik,fasigin,fasigyn,glongyn,haisigyn,isotinidazole,pletil,protozol,simplotan,sorquetan,symplotan,tindamax,tindazole,tinidazol,tinidazolum,tricolam,trimonase</t>
         </is>
       </c>
       <c r="J473">
@@ -29602,7 +29602,7 @@
       </c>
       <c r="I474" t="inlineStr">
         <is>
-          <t>amixyl,datanil,disocarban,disoxyl,isoxyl,thiocarlide,tiocarlid,tiocarlida,tiocarlidum</t>
+          <t>aethoksid,aethoxyd,aethoxydum,amixyl,datanil,disocarban,disoxyl,ethoxide,ethoxyd,etocarlid,etocarlida,etocarlide,etocarlidum,etoksid,thiocarlide,tiocarlid,tiocarlida,tiocarlidum</t>
         </is>
       </c>
       <c r="J474">
@@ -29662,7 +29662,7 @@
       </c>
       <c r="I475" t="inlineStr">
         <is>
-          <t>clorurodetiodonio,tiodoniichloridum,tiodoniumchloride</t>
+          <t>tiodonium</t>
         </is>
       </c>
       <c r="J475" t="e">
@@ -29720,7 +29720,7 @@
       </c>
       <c r="I476" t="inlineStr">
         <is>
-          <t>tioxacine,tioxacino,tioxacinum,tioxicacid</t>
+          <t>tioxacine,tioxacino,tioxacinum</t>
         </is>
       </c>
       <c r="J476" t="e">
@@ -29778,7 +29778,7 @@
       </c>
       <c r="I477" t="inlineStr">
         <is>
-          <t>ntzdes</t>
+          <t/>
         </is>
       </c>
       <c r="J477" t="e">
@@ -29840,7 +29840,7 @@
       </c>
       <c r="I478" t="inlineStr">
         <is>
-          <t>bethkis,brulamycin,deoxykanamycinb,distobram,gernebcin,gotabiotic,kitabis,kitabispak,nebcin,nebicin,nebramycin,nebramycinvi,obramycin,sybryx,tenebrimycin,tenemycin,tobacin,tobipodhaler,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycinbase,tobramycine,tobramycinsulfate,tobramycinum,tobrased,tobrasone,tobrex</t>
+          <t>aktob,bethkis,distobram,gotabiotic,kitabis,nebcin,nebicin,nebramycin,obramycin,tenebrimycin,tenemycin,tobacin,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycine,tobramycinum,tobrased,tobrex</t>
         </is>
       </c>
       <c r="J478" t="e">
@@ -30022,7 +30022,7 @@
       </c>
       <c r="I481" t="inlineStr">
         <is>
-          <t>abaprim,alprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacterial,bacticel,bactifor,bactin,bactoprim,bactramin,bactrim,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,colizoleds,conprim,cotrimel,cotrimoxizole,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,idotrim,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lagatrimforte,lastrim,lescot,methoprim,metoprim,monoprim,monotrim,monotrimin,novotrimel,omstat,oraprim,pancidim,polytrim,priloprim,primosept,primsol,proloprim,protrin,purbal,resprim,resprimforte,roubac,roubal,salvatrim,septrinds,septrinforte,septrins,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfamethoprim,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,tmpsmx,toprim,trimanyl,trimethioprim,trimethopim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexazole,trimexol,trimezol,trimogal,trimono,trimopan,trimpex,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
+          <t>abaprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacin,bacta,bacterial,bacticel,bactifor,bactoprim,bactramin,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,conprim,cotrimel,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,futin,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lastrim,lescot,metoprim,monoprim,monotrim,monotrimin,novotrimel,omstat,pancidim,proloprim,protrin,purbal,resprim,roubac,roubal,salvatrim,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,toprim,trimethioprim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexol,trimezol,trimogal,trimono,trimopan,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
         </is>
       </c>
       <c r="J481">
@@ -30088,7 +30088,7 @@
       </c>
       <c r="I482" t="inlineStr">
         <is>
-          <t>abacin,abactrim,agoprim,alfatrim,aposulfatrim,bacteral,bacterialforte,bactilen,bactiver,bacton,bactoreduct,bactrim,bactrimds,bactrimel,bactrimforte,bactrimpediatric,bactrizol,bactromin,bactropin,baktar,belcomycine,berlocid,bibacrim,biseptol,chemitrim,chemotrim,ciplin,colimycin,colimycinsulphate,colisticin,colistimethate,colistimethatesodium,colistinsulfate,colistinsulphate,colomycin,colymycin,cotribene,cotrimaxazol,cotrimazole,cotrimds,cotrimeurho,cotrimhexal,cotrimholsen,cotrimlut,cotrimoxazol,cotrimoxazolal,cotrimoxazole,cotrimstada,cotriver,dibaprim,drylin,duratrimet,eltrianyl,escoprim,esteprim,eusaprim,fectrim,gantaprim,gantaprin,gantrim,groprim,helveprim,imexim,jenamoxazol,kemoprim,kepinol,kepinolforte,laratrim,linaris,maxtrim,microtrim,microtrimforte,mikrosid,momentol,oecotrim,oriprim,oxaprim,pantoprim,polymyxine,polymyxinesulfate,primazole,promixin,septra,septrads,septragrape,septrim,septrin,servitrim,sigaprim,sigaprin,sulfatrimpediatric,sulfotrim,sulfotrimin,sulmeprimpediatric,sulprim,sumetrolim,supracombin,suprim,tacumil,teleprim,teleprin,thiocuran,totazina,tribakin,trifen,trigonyl,trimesulf,trimethocomp,trimethoprimsulfa,trimetoger,trimexazol,trimforte,trimosulfa,uroplus,uroplusds,uroplusss</t>
+          <t>abacin,abactrim,agoprim,alfatrim,aposulfatrim,bacteral,bactilen,bactiver,bacton,bactoreduct,bactrim,bactrizol,bactromin,bactropin,baktar,benzenesulfonamide,berlocid,bibacrim,biseptol,centran,centrin,chemitrim,chemotrim,ciplin,comox,cotribene,cotrim,cotrimhexal,cotrimoxazol,cotrimoxazole,cotrimstada,cotriver,dibaprim,drylin,duratrimet,eltrianyl,escoprim,eslectin,esteprim,eusaprim,fectrim,gamazole,gantanol,gantaprim,gantaprin,gantrim,groprim,helveprim,imexim,insozalin,jenamoxazol,kemoprim,kepinol,laratrim,linaris,maxtrim,metoxal,microtrim,mikrosid,momentol,nopil,oecotrim,omsat,oriprim,oxaprim,pantoprim,potrox,primazole,radonil,septra,septrim,servitrim,sigaprim,sigaprin,sulfatrim,sulfotrim,sulfotrimin,sulmeprim,sulprim,sumetrolim,supracombin,suprim,tacumil,teleprim,teleprin,thiocuran,tribakin,trifen,trigonyl,trimedin,trimesulf,trimethoprimsulfa,trimetoger,trimexazol,trimezole,trimforte,trimosulfa,uroplus</t>
         </is>
       </c>
       <c r="J482" t="e">
@@ -30150,7 +30150,7 @@
       </c>
       <c r="I483" t="inlineStr">
         <is>
-          <t>acetyloleandomycin,aovine,cyclamycin,evramicina,matromicina,matromycint,micotil,oleandocetine,tao,treolmicina,tribiocillina,triocetin,triolan,troleandomicina,troleandomycine,troleandomycinum,viamicina,wytrion</t>
+          <t>aovine,cyclamycin,evramicina,matromicina,oleandocetin,oleandocetine,tekmisin,treolmicina,tribiocillina,triocetin,triolan,troleandomicina,troleandomycine,troleandomycinum,viamicina,wytrion</t>
         </is>
       </c>
       <c r="J483">
@@ -30210,7 +30210,7 @@
       </c>
       <c r="I484" t="inlineStr">
         <is>
-          <t>rubidiumnitrate,trospectinomycin,trospectomicina,trospectomycine,trospectomycinum</t>
+          <t>trospectinomycin,trospectomicina,trospectomycine,trospectomycinum</t>
         </is>
       </c>
       <c r="J484" t="e">
@@ -30272,7 +30272,7 @@
       </c>
       <c r="I485" t="inlineStr">
         <is>
-          <t>trovan</t>
+          <t>trovan,turvel</t>
         </is>
       </c>
       <c r="J485">
@@ -30334,7 +30334,7 @@
       </c>
       <c r="I486" t="inlineStr">
         <is>
-          <t>draxxin,tulathrmycina,tulathromycina</t>
+          <t>arovyn,draxxin,increxxa,macrosyn,tulieve,tulissin</t>
         </is>
       </c>
       <c r="J486" t="e">
@@ -30392,7 +30392,7 @@
       </c>
       <c r="I487" t="inlineStr">
         <is>
-          <t>fradizine,tilosina,tylocine,tylosina,tylosine,tylosinum</t>
+          <t>fradizine,tilosina,tylan,tylocine,tylosine,tylosinum,vubityl</t>
         </is>
       </c>
       <c r="J487" t="e">
@@ -30450,7 +30450,7 @@
       </c>
       <c r="I488" t="inlineStr">
         <is>
-          <t/>
+          <t>aivlosin</t>
         </is>
       </c>
       <c r="J488" t="e">
@@ -30570,7 +30570,7 @@
       </c>
       <c r="I490" t="inlineStr">
         <is>
-          <t>vancocin,vancocinhcl,vancoled,vancomicina,vancomycine,vancomycinhcl,vancomycinum,vancor,viomycinderivative</t>
+          <t>vancocin,vancoled,vancomicina,vancomycine,vancomycinum</t>
         </is>
       </c>
       <c r="J490">
@@ -30690,7 +30690,7 @@
       </c>
       <c r="I492" t="inlineStr">
         <is>
-          <t>celiomycin,florimycin,floromycin,tuberactinomycinb,vinacetina,vioactane,viomicina,viomycine,viomycinum</t>
+          <t>florimycin,floromycin,vioactane,viocin,viomicin,viomicina,viomycine,viomycinum</t>
         </is>
       </c>
       <c r="J492" t="e">
@@ -30748,7 +30748,7 @@
       </c>
       <c r="I493" t="inlineStr">
         <is>
-          <t>eskalin,eskalinv,micamicina,mikamycin,mikamycine,mikamycinum,ostreogricina,ostreogrycin,ostreogrycine,ostreogrycinum,pristinamicina,pristinamycine,pristinamycinum,pyostacine,stafac,stafytracine,staphylomycin,stapyocine,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamicina,virginiamycin,virginiamycina,virginiamycinum</t>
+          <t/>
         </is>
       </c>
       <c r="J493" t="e">
@@ -30810,7 +30810,7 @@
       </c>
       <c r="I494" t="inlineStr">
         <is>
-          <t>pfizer,vfendiv,voriconazol,voriconazolevfend,voriconazolum,voriconzole,vorikonazole</t>
+          <t>vfend,voriconazol,voriconazolum,voriconzole,vorikonazole</t>
         </is>
       </c>
       <c r="J494">
@@ -30934,7 +30934,7 @@
       </c>
       <c r="I496" t="inlineStr">
         <is>
-          <t/>
+          <t>zidebactamsalt</t>
         </is>
       </c>
       <c r="J496" t="e">

</xml_diff>